<commit_message>
data on map 4
</commit_message>
<xml_diff>
--- a/python_code/data/map 3/all_agents_score.xlsx
+++ b/python_code/data/map 3/all_agents_score.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F190"/>
+  <dimension ref="A1:F199"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1231,44 +1231,44 @@
     <row r="34">
       <c r="A34" s="1" t="inlineStr">
         <is>
-          <t>-Mr4SdCNCuYdvb9_MpJ6</t>
+          <t>-Mr4SX2AqADEfXMoU2vJ</t>
         </is>
       </c>
       <c r="B34" t="n">
-        <v>0.71</v>
+        <v>0.5199999999999999</v>
       </c>
       <c r="C34" t="n">
-        <v>-0.37</v>
+        <v>0.3</v>
       </c>
       <c r="D34" t="n">
-        <v>0.71</v>
+        <v>0.57</v>
       </c>
       <c r="E34" t="n">
-        <v>-0.12</v>
+        <v>0.5</v>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>selfish</t>
+          <t>random</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="inlineStr">
         <is>
-          <t>-Mr4Sds3e3LNtngNiiYM</t>
+          <t>-Mr4SdCNCuYdvb9_MpJ6</t>
         </is>
       </c>
       <c r="B35" t="n">
-        <v>1.08</v>
+        <v>0.71</v>
       </c>
       <c r="C35" t="n">
-        <v>-0.5</v>
+        <v>-0.37</v>
       </c>
       <c r="D35" t="n">
-        <v>1.08</v>
+        <v>0.71</v>
       </c>
       <c r="E35" t="n">
-        <v>-0.25</v>
+        <v>-0.12</v>
       </c>
       <c r="F35" t="inlineStr">
         <is>
@@ -1279,68 +1279,68 @@
     <row r="36">
       <c r="A36" s="1" t="inlineStr">
         <is>
-          <t>-Mr4SfOEa5KV0VxFPQsF</t>
+          <t>-Mr4Sds3e3LNtngNiiYM</t>
         </is>
       </c>
       <c r="B36" t="n">
-        <v>0.18</v>
+        <v>1.08</v>
       </c>
       <c r="C36" t="n">
-        <v>0.17</v>
+        <v>-0.5</v>
       </c>
       <c r="D36" t="n">
-        <v>0.28</v>
+        <v>1.08</v>
       </c>
       <c r="E36" t="n">
-        <v>0.32</v>
+        <v>-0.25</v>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>random</t>
+          <t>selfish</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="inlineStr">
         <is>
-          <t>-Mr4SoBXnG5uBK8X318c</t>
+          <t>-Mr4SfOEa5KV0VxFPQsF</t>
         </is>
       </c>
       <c r="B37" t="n">
-        <v>0.65</v>
+        <v>0.18</v>
       </c>
       <c r="C37" t="n">
-        <v>0.65</v>
+        <v>0.17</v>
       </c>
       <c r="D37" t="n">
-        <v>0.75</v>
+        <v>0.28</v>
       </c>
       <c r="E37" t="n">
-        <v>0.8</v>
+        <v>0.32</v>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>closest</t>
+          <t>random</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="inlineStr">
         <is>
-          <t>-Mr4Stb5V_DdbhxE2GtG</t>
+          <t>-Mr4SoBXnG5uBK8X318c</t>
         </is>
       </c>
       <c r="B38" t="n">
         <v>0.65</v>
       </c>
       <c r="C38" t="n">
-        <v>0.6</v>
+        <v>0.65</v>
       </c>
       <c r="D38" t="n">
         <v>0.75</v>
       </c>
       <c r="E38" t="n">
-        <v>0.75</v>
+        <v>0.8</v>
       </c>
       <c r="F38" t="inlineStr">
         <is>
@@ -1351,116 +1351,116 @@
     <row r="39">
       <c r="A39" s="1" t="inlineStr">
         <is>
-          <t>-Mr4SvGqJkDMn6IilyXX</t>
+          <t>-Mr4SpmghQ3iMykH6rlt</t>
         </is>
       </c>
       <c r="B39" t="n">
-        <v>-0.1</v>
+        <v>1.22</v>
       </c>
       <c r="C39" t="n">
-        <v>-0.5</v>
+        <v>0.09999999999999998</v>
       </c>
       <c r="D39" t="n">
-        <v>-0.1</v>
+        <v>1.22</v>
       </c>
       <c r="E39" t="n">
-        <v>-0.25</v>
+        <v>0.35</v>
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>random</t>
+          <t>selfish</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="1" t="inlineStr">
         <is>
-          <t>-Mr4SzmsaQRIdsXjl6iK</t>
+          <t>-Mr4Sq_x7xVa1E2B2FaR</t>
         </is>
       </c>
       <c r="B40" t="n">
         <v>0.25</v>
       </c>
       <c r="C40" t="n">
-        <v>0.7</v>
+        <v>0.3</v>
       </c>
       <c r="D40" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="E40" t="n">
         <v>0.5</v>
       </c>
-      <c r="E40" t="n">
-        <v>0.7</v>
-      </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>TSP</t>
+          <t>farthest</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="1" t="inlineStr">
         <is>
-          <t>-Mr4T-JNf7gFH1lSZR71</t>
+          <t>-Mr4StVOAeBvEVeHeRsH</t>
         </is>
       </c>
       <c r="B41" t="n">
-        <v>1.25</v>
+        <v>0.43</v>
       </c>
       <c r="C41" t="n">
-        <v>0.29</v>
+        <v>-0.2</v>
       </c>
       <c r="D41" t="n">
-        <v>1.25</v>
+        <v>0.43</v>
       </c>
       <c r="E41" t="n">
-        <v>0.54</v>
+        <v>0.05</v>
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>selfish</t>
+          <t>random</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="1" t="inlineStr">
         <is>
-          <t>-Mr4T8dkYvS00oNjILmt</t>
+          <t>-Mr4Stb5V_DdbhxE2GtG</t>
         </is>
       </c>
       <c r="B42" t="n">
-        <v>0.4</v>
+        <v>0.65</v>
       </c>
       <c r="C42" t="n">
-        <v>0.4</v>
+        <v>0.6</v>
       </c>
       <c r="D42" t="n">
-        <v>0.45</v>
+        <v>0.75</v>
       </c>
       <c r="E42" t="n">
-        <v>0.6</v>
+        <v>0.75</v>
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>farthest</t>
+          <t>closest</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="1" t="inlineStr">
         <is>
-          <t>-Mr4T9ZoabzTK-m8YDAN</t>
+          <t>-Mr4SvGqJkDMn6IilyXX</t>
         </is>
       </c>
       <c r="B43" t="n">
-        <v>0.52</v>
+        <v>-0.1</v>
       </c>
       <c r="C43" t="n">
-        <v>0.2</v>
+        <v>-0.5</v>
       </c>
       <c r="D43" t="n">
-        <v>0.52</v>
+        <v>-0.1</v>
       </c>
       <c r="E43" t="n">
-        <v>0.45</v>
+        <v>-0.25</v>
       </c>
       <c r="F43" t="inlineStr">
         <is>
@@ -1471,68 +1471,68 @@
     <row r="44">
       <c r="A44" s="1" t="inlineStr">
         <is>
-          <t>-Mr4TCM3hSkdje5YTSxx</t>
+          <t>-Mr4SzmsaQRIdsXjl6iK</t>
         </is>
       </c>
       <c r="B44" t="n">
-        <v>0.4</v>
+        <v>0.25</v>
       </c>
       <c r="C44" t="n">
-        <v>0.4</v>
+        <v>0.7</v>
       </c>
       <c r="D44" t="n">
-        <v>0.45</v>
+        <v>0.5</v>
       </c>
       <c r="E44" t="n">
-        <v>0.6</v>
+        <v>0.7</v>
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>farthest</t>
+          <t>TSP</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="1" t="inlineStr">
         <is>
-          <t>-Mr4TNp363LOScZ9hwXJ</t>
+          <t>-Mr4T-JNf7gFH1lSZR71</t>
         </is>
       </c>
       <c r="B45" t="n">
-        <v>0.65</v>
+        <v>1.25</v>
       </c>
       <c r="C45" t="n">
-        <v>0.75</v>
+        <v>0.29</v>
       </c>
       <c r="D45" t="n">
-        <v>0.75</v>
+        <v>1.25</v>
       </c>
       <c r="E45" t="n">
-        <v>0.9</v>
+        <v>0.54</v>
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>closest</t>
+          <t>selfish</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="1" t="inlineStr">
         <is>
-          <t>-Mr4TOMJZVOFvVPQVDT_</t>
+          <t>-Mr4T8dkYvS00oNjILmt</t>
         </is>
       </c>
       <c r="B46" t="n">
-        <v>0.25</v>
+        <v>0.4</v>
       </c>
       <c r="C46" t="n">
-        <v>0.29</v>
+        <v>0.4</v>
       </c>
       <c r="D46" t="n">
-        <v>0.3</v>
+        <v>0.45</v>
       </c>
       <c r="E46" t="n">
-        <v>0.49</v>
+        <v>0.6</v>
       </c>
       <c r="F46" t="inlineStr">
         <is>
@@ -1543,20 +1543,20 @@
     <row r="47">
       <c r="A47" s="1" t="inlineStr">
         <is>
-          <t>-Mr4TSTAmBR0HW8puqd8</t>
+          <t>-Mr4T9ZoabzTK-m8YDAN</t>
         </is>
       </c>
       <c r="B47" t="n">
-        <v>0.6899999999999999</v>
+        <v>0.52</v>
       </c>
       <c r="C47" t="n">
-        <v>0.4</v>
+        <v>0.2</v>
       </c>
       <c r="D47" t="n">
-        <v>0.74</v>
+        <v>0.52</v>
       </c>
       <c r="E47" t="n">
-        <v>0.6</v>
+        <v>0.45</v>
       </c>
       <c r="F47" t="inlineStr">
         <is>
@@ -1567,44 +1567,44 @@
     <row r="48">
       <c r="A48" s="1" t="inlineStr">
         <is>
-          <t>-Mr4TSpiZH6dTCPh0LlE</t>
+          <t>-Mr4T9nAc23w1GQ7IDSy</t>
         </is>
       </c>
       <c r="B48" t="n">
-        <v>0.36</v>
+        <v>0.35</v>
       </c>
       <c r="C48" t="n">
-        <v>0.3</v>
+        <v>0.4</v>
       </c>
       <c r="D48" t="n">
-        <v>0.41</v>
+        <v>0.45</v>
       </c>
       <c r="E48" t="n">
-        <v>0.5</v>
+        <v>0.55</v>
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>random</t>
+          <t>farthest</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="1" t="inlineStr">
         <is>
-          <t>-Mr4TbrlbYAuDO9jVXM1</t>
+          <t>-Mr4TA4uTRX9CK1PKDNi</t>
         </is>
       </c>
       <c r="B49" t="n">
-        <v>0.85</v>
+        <v>0.35</v>
       </c>
       <c r="C49" t="n">
-        <v>0.7999999999999999</v>
+        <v>0.3</v>
       </c>
       <c r="D49" t="n">
-        <v>0.95</v>
+        <v>0.45</v>
       </c>
       <c r="E49" t="n">
-        <v>0.95</v>
+        <v>0.45</v>
       </c>
       <c r="F49" t="inlineStr">
         <is>
@@ -1615,44 +1615,44 @@
     <row r="50">
       <c r="A50" s="1" t="inlineStr">
         <is>
-          <t>-Mr4Tkudz1r4_hZxtwny</t>
+          <t>-Mr4TCM3hSkdje5YTSxx</t>
         </is>
       </c>
       <c r="B50" t="n">
-        <v>0.34</v>
+        <v>0.4</v>
       </c>
       <c r="C50" t="n">
-        <v>0.09999999999999998</v>
+        <v>0.4</v>
       </c>
       <c r="D50" t="n">
-        <v>0.34</v>
+        <v>0.45</v>
       </c>
       <c r="E50" t="n">
-        <v>0.35</v>
+        <v>0.6</v>
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>random</t>
+          <t>farthest</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="1" t="inlineStr">
         <is>
-          <t>-Mr4U22_owhdQn8fPo2q</t>
+          <t>-Mr4TNp363LOScZ9hwXJ</t>
         </is>
       </c>
       <c r="B51" t="n">
-        <v>0.45</v>
+        <v>0.65</v>
       </c>
       <c r="C51" t="n">
-        <v>1.17</v>
+        <v>0.75</v>
       </c>
       <c r="D51" t="n">
-        <v>0.65</v>
+        <v>0.75</v>
       </c>
       <c r="E51" t="n">
-        <v>1.22</v>
+        <v>0.9</v>
       </c>
       <c r="F51" t="inlineStr">
         <is>
@@ -1663,164 +1663,164 @@
     <row r="52">
       <c r="A52" s="1" t="inlineStr">
         <is>
-          <t>-Mr4UCcJuMhGpOxwolOa</t>
+          <t>-Mr4TOMJZVOFvVPQVDT_</t>
         </is>
       </c>
       <c r="B52" t="n">
-        <v>1.05</v>
+        <v>0.25</v>
       </c>
       <c r="C52" t="n">
-        <v>0.9999999999999999</v>
+        <v>0.29</v>
       </c>
       <c r="D52" t="n">
-        <v>1.15</v>
+        <v>0.3</v>
       </c>
       <c r="E52" t="n">
-        <v>1.15</v>
+        <v>0.49</v>
       </c>
       <c r="F52" t="inlineStr">
         <is>
-          <t>TSP</t>
+          <t>farthest</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="1" t="inlineStr">
         <is>
-          <t>-Mr4UJ-FP6wX5rEnoKDQ</t>
+          <t>-Mr4TQDA7yqwKG2GDHPl</t>
         </is>
       </c>
       <c r="B53" t="n">
-        <v>0.85</v>
+        <v>0.45</v>
       </c>
       <c r="C53" t="n">
-        <v>0.7999999999999999</v>
+        <v>0.4</v>
       </c>
       <c r="D53" t="n">
-        <v>0.95</v>
+        <v>0.65</v>
       </c>
       <c r="E53" t="n">
-        <v>0.95</v>
+        <v>0.5</v>
       </c>
       <c r="F53" t="inlineStr">
         <is>
-          <t>TSP</t>
+          <t>closest</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="1" t="inlineStr">
         <is>
-          <t>-Mr4UMneVuEOivyI4gZA</t>
+          <t>-Mr4TSSaKuIDrhogt0-Y</t>
         </is>
       </c>
       <c r="B54" t="n">
-        <v>-0.02</v>
+        <v>0.85</v>
       </c>
       <c r="C54" t="n">
-        <v>-1.01</v>
+        <v>0.7999999999999999</v>
       </c>
       <c r="D54" t="n">
-        <v>-0.02</v>
+        <v>0.95</v>
       </c>
       <c r="E54" t="n">
-        <v>-0.76</v>
+        <v>0.95</v>
       </c>
       <c r="F54" t="inlineStr">
         <is>
-          <t>selfish</t>
+          <t>TSP</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="1" t="inlineStr">
         <is>
-          <t>-Mr4UNdvlMU8SvAcB4jY</t>
+          <t>-Mr4TSTAmBR0HW8puqd8</t>
         </is>
       </c>
       <c r="B55" t="n">
+        <v>0.6899999999999999</v>
+      </c>
+      <c r="C55" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="D55" t="n">
+        <v>0.74</v>
+      </c>
+      <c r="E55" t="n">
         <v>0.6</v>
       </c>
-      <c r="C55" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="D55" t="n">
-        <v>0.7</v>
-      </c>
-      <c r="E55" t="n">
-        <v>0.65</v>
-      </c>
       <c r="F55" t="inlineStr">
         <is>
-          <t>closest</t>
+          <t>random</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="1" t="inlineStr">
         <is>
-          <t>-Mr4UOt_rLMvfCGidXCV</t>
+          <t>-Mr4TSpiZH6dTCPh0LlE</t>
         </is>
       </c>
       <c r="B56" t="n">
-        <v>1.17</v>
+        <v>0.36</v>
       </c>
       <c r="C56" t="n">
-        <v>-0.15</v>
+        <v>0.3</v>
       </c>
       <c r="D56" t="n">
-        <v>1.17</v>
+        <v>0.41</v>
       </c>
       <c r="E56" t="n">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
       <c r="F56" t="inlineStr">
         <is>
-          <t>selfish</t>
+          <t>random</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="1" t="inlineStr">
         <is>
-          <t>-Mr4UYHcrL76eIOnb22w</t>
+          <t>-Mr4TbrlbYAuDO9jVXM1</t>
         </is>
       </c>
       <c r="B57" t="n">
-        <v>1.16</v>
+        <v>0.85</v>
       </c>
       <c r="C57" t="n">
-        <v>0.03999999999999998</v>
+        <v>0.7999999999999999</v>
       </c>
       <c r="D57" t="n">
-        <v>1.16</v>
+        <v>0.95</v>
       </c>
       <c r="E57" t="n">
-        <v>0.29</v>
+        <v>0.95</v>
       </c>
       <c r="F57" t="inlineStr">
         <is>
-          <t>selfish</t>
+          <t>TSP</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="1" t="inlineStr">
         <is>
-          <t>-Mr4UbgWePKxAMky1vMe</t>
+          <t>-Mr4TdH6U1XoC9dOKdFF</t>
         </is>
       </c>
       <c r="B58" t="n">
-        <v>0.35</v>
+        <v>0.45</v>
       </c>
       <c r="C58" t="n">
-        <v>0.35</v>
+        <v>0.45</v>
       </c>
       <c r="D58" t="n">
-        <v>0.45</v>
+        <v>0.5</v>
       </c>
       <c r="E58" t="n">
-        <v>0.5</v>
+        <v>0.65</v>
       </c>
       <c r="F58" t="inlineStr">
         <is>
@@ -1831,236 +1831,236 @@
     <row r="59">
       <c r="A59" s="1" t="inlineStr">
         <is>
-          <t>-Mr4Ud8lbqJ_NmwqcuVd</t>
+          <t>-Mr4Tkudz1r4_hZxtwny</t>
         </is>
       </c>
       <c r="B59" t="n">
-        <v>1.12</v>
+        <v>0.34</v>
       </c>
       <c r="C59" t="n">
-        <v>-0.2</v>
+        <v>0.09999999999999998</v>
       </c>
       <c r="D59" t="n">
-        <v>1.12</v>
+        <v>0.34</v>
       </c>
       <c r="E59" t="n">
-        <v>0.05</v>
+        <v>0.35</v>
       </c>
       <c r="F59" t="inlineStr">
         <is>
-          <t>selfish</t>
+          <t>random</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="1" t="inlineStr">
         <is>
-          <t>-Mr4UjxGLiaOpLnJm4Ij</t>
+          <t>-Mr4TsYTLOr9GP4423xa</t>
         </is>
       </c>
       <c r="B60" t="n">
-        <v>1.05</v>
+        <v>0.6</v>
       </c>
       <c r="C60" t="n">
-        <v>0.9999999999999999</v>
+        <v>0.6</v>
       </c>
       <c r="D60" t="n">
-        <v>1.15</v>
+        <v>0.7</v>
       </c>
       <c r="E60" t="n">
-        <v>1.15</v>
+        <v>0.75</v>
       </c>
       <c r="F60" t="inlineStr">
         <is>
-          <t>TSP</t>
+          <t>closest</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" s="1" t="inlineStr">
         <is>
-          <t>-Mr4Ut1L-oObBWTyF2pw</t>
+          <t>-Mr4Tt7ZuGN2qc9kf-Tt</t>
         </is>
       </c>
       <c r="B61" t="n">
-        <v>0.6</v>
+        <v>-0.44</v>
       </c>
       <c r="C61" t="n">
-        <v>0.65</v>
+        <v>-0.1</v>
       </c>
       <c r="D61" t="n">
-        <v>0.75</v>
+        <v>-0.44</v>
       </c>
       <c r="E61" t="n">
-        <v>0.75</v>
+        <v>0.15</v>
       </c>
       <c r="F61" t="inlineStr">
         <is>
-          <t>closest</t>
+          <t>random</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" s="1" t="inlineStr">
         <is>
-          <t>-Mr4UxN0e26HH3gDWNqU</t>
+          <t>-Mr4U22_owhdQn8fPo2q</t>
         </is>
       </c>
       <c r="B62" t="n">
-        <v>0.55</v>
+        <v>0.45</v>
       </c>
       <c r="C62" t="n">
-        <v>0.15</v>
+        <v>1.17</v>
       </c>
       <c r="D62" t="n">
-        <v>0.55</v>
+        <v>0.65</v>
       </c>
       <c r="E62" t="n">
-        <v>0.4</v>
+        <v>1.22</v>
       </c>
       <c r="F62" t="inlineStr">
         <is>
-          <t>random</t>
+          <t>closest</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" s="1" t="inlineStr">
         <is>
-          <t>-Mr4V2R-FuAlrB31ccSL</t>
+          <t>-Mr4U6QWerzTJfKbodpv</t>
         </is>
       </c>
       <c r="B63" t="n">
-        <v>0.5499999999999999</v>
+        <v>0.36</v>
       </c>
       <c r="C63" t="n">
-        <v>0.59</v>
+        <v>0.2</v>
       </c>
       <c r="D63" t="n">
-        <v>0.7</v>
+        <v>0.36</v>
       </c>
       <c r="E63" t="n">
-        <v>0.6899999999999999</v>
+        <v>0.45</v>
       </c>
       <c r="F63" t="inlineStr">
         <is>
-          <t>closest</t>
+          <t>random</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" s="1" t="inlineStr">
         <is>
-          <t>-Mr4VCw2qL_Bo6gK2Gde</t>
+          <t>-Mr4UAlobBG3uxVuiRMk</t>
         </is>
       </c>
       <c r="B64" t="n">
-        <v>0.75</v>
+        <v>0.41</v>
       </c>
       <c r="C64" t="n">
-        <v>0.7</v>
+        <v>0.15</v>
       </c>
       <c r="D64" t="n">
-        <v>0.85</v>
+        <v>0.41</v>
       </c>
       <c r="E64" t="n">
-        <v>0.85</v>
+        <v>0.4</v>
       </c>
       <c r="F64" t="inlineStr">
         <is>
-          <t>closest</t>
+          <t>random</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" s="1" t="inlineStr">
         <is>
-          <t>-Mr4VHIAFIXo8DhoUVKp</t>
+          <t>-Mr4UCcJuMhGpOxwolOa</t>
         </is>
       </c>
       <c r="B65" t="n">
-        <v>0.45</v>
+        <v>1.05</v>
       </c>
       <c r="C65" t="n">
-        <v>0.77</v>
+        <v>0.9999999999999999</v>
       </c>
       <c r="D65" t="n">
-        <v>0.6</v>
+        <v>1.15</v>
       </c>
       <c r="E65" t="n">
-        <v>0.87</v>
+        <v>1.15</v>
       </c>
       <c r="F65" t="inlineStr">
         <is>
-          <t>closest</t>
+          <t>TSP</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" s="1" t="inlineStr">
         <is>
-          <t>-Mr4VKFfLDB45xOtua-M</t>
+          <t>-Mr4UJ-FP6wX5rEnoKDQ</t>
         </is>
       </c>
       <c r="B66" t="n">
-        <v>0.86</v>
+        <v>0.85</v>
       </c>
       <c r="C66" t="n">
-        <v>0.09999999999999998</v>
+        <v>0.7999999999999999</v>
       </c>
       <c r="D66" t="n">
-        <v>0.96</v>
+        <v>0.95</v>
       </c>
       <c r="E66" t="n">
-        <v>0.25</v>
+        <v>0.95</v>
       </c>
       <c r="F66" t="inlineStr">
         <is>
-          <t>farthest</t>
+          <t>TSP</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" s="1" t="inlineStr">
         <is>
-          <t>-Mr4VRV9hRV-yTio4Z7s</t>
+          <t>-Mr4ULm2vCu_AqNvourR</t>
         </is>
       </c>
       <c r="B67" t="n">
-        <v>1.12</v>
+        <v>0.54</v>
       </c>
       <c r="C67" t="n">
-        <v>-0.3</v>
+        <v>0.3</v>
       </c>
       <c r="D67" t="n">
-        <v>1.12</v>
+        <v>0.54</v>
       </c>
       <c r="E67" t="n">
-        <v>-0.05</v>
+        <v>0.55</v>
       </c>
       <c r="F67" t="inlineStr">
         <is>
-          <t>selfish</t>
+          <t>random</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" s="1" t="inlineStr">
         <is>
-          <t>-Mr4VrgeSScBxw-VOkCj</t>
+          <t>-Mr4UMneVuEOivyI4gZA</t>
         </is>
       </c>
       <c r="B68" t="n">
-        <v>1.26</v>
+        <v>-0.02</v>
       </c>
       <c r="C68" t="n">
-        <v>0.3</v>
+        <v>-1.01</v>
       </c>
       <c r="D68" t="n">
-        <v>1.26</v>
+        <v>-0.02</v>
       </c>
       <c r="E68" t="n">
-        <v>0.55</v>
+        <v>-0.76</v>
       </c>
       <c r="F68" t="inlineStr">
         <is>
@@ -2071,140 +2071,140 @@
     <row r="69">
       <c r="A69" s="1" t="inlineStr">
         <is>
-          <t>-Mr4VvMxhAb1yIPOQ0tV</t>
+          <t>-Mr4UNdvlMU8SvAcB4jY</t>
         </is>
       </c>
       <c r="B69" t="n">
-        <v>0.71</v>
+        <v>0.6</v>
       </c>
       <c r="C69" t="n">
-        <v>0.35</v>
+        <v>0.5</v>
       </c>
       <c r="D69" t="n">
-        <v>0.76</v>
+        <v>0.7</v>
       </c>
       <c r="E69" t="n">
-        <v>0.55</v>
+        <v>0.65</v>
       </c>
       <c r="F69" t="inlineStr">
         <is>
-          <t>random</t>
+          <t>closest</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" s="1" t="inlineStr">
         <is>
-          <t>-Mr4VyzMcKi-TVbEWVbs</t>
+          <t>-Mr4UOt_rLMvfCGidXCV</t>
         </is>
       </c>
       <c r="B70" t="n">
-        <v>-0.3</v>
+        <v>1.17</v>
       </c>
       <c r="C70" t="n">
-        <v>0.22</v>
+        <v>-0.15</v>
       </c>
       <c r="D70" t="n">
-        <v>-0.25</v>
+        <v>1.17</v>
       </c>
       <c r="E70" t="n">
-        <v>0.42</v>
+        <v>0.1</v>
       </c>
       <c r="F70" t="inlineStr">
         <is>
-          <t>farthest</t>
+          <t>selfish</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" s="1" t="inlineStr">
         <is>
-          <t>-Mr4Vzctm_Axuz_zPELo</t>
+          <t>-Mr4UYHcrL76eIOnb22w</t>
         </is>
       </c>
       <c r="B71" t="n">
-        <v>0.35</v>
+        <v>1.16</v>
       </c>
       <c r="C71" t="n">
-        <v>0.35</v>
+        <v>0.03999999999999998</v>
       </c>
       <c r="D71" t="n">
-        <v>0.45</v>
+        <v>1.16</v>
       </c>
       <c r="E71" t="n">
-        <v>0.5</v>
+        <v>0.29</v>
       </c>
       <c r="F71" t="inlineStr">
         <is>
-          <t>farthest</t>
+          <t>selfish</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" s="1" t="inlineStr">
         <is>
-          <t>-Mr4W4EWZ2YgC3PURuQT</t>
+          <t>-Mr4UaF33TWgy-KKFy78</t>
         </is>
       </c>
       <c r="B72" t="n">
-        <v>0.15</v>
+        <v>1.16</v>
       </c>
       <c r="C72" t="n">
-        <v>0.35</v>
+        <v>-0.2</v>
       </c>
       <c r="D72" t="n">
-        <v>0.2</v>
+        <v>1.16</v>
       </c>
       <c r="E72" t="n">
-        <v>0.55</v>
+        <v>0.05</v>
       </c>
       <c r="F72" t="inlineStr">
         <is>
-          <t>farthest</t>
+          <t>selfish</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" s="1" t="inlineStr">
         <is>
-          <t>-Mr4WEHdyw5TmHtu1p8h</t>
+          <t>-Mr4UbgWePKxAMky1vMe</t>
         </is>
       </c>
       <c r="B73" t="n">
-        <v>0.91</v>
+        <v>0.35</v>
       </c>
       <c r="C73" t="n">
-        <v>-0.04999999999999999</v>
+        <v>0.35</v>
       </c>
       <c r="D73" t="n">
-        <v>0.91</v>
+        <v>0.45</v>
       </c>
       <c r="E73" t="n">
-        <v>0.2</v>
+        <v>0.5</v>
       </c>
       <c r="F73" t="inlineStr">
         <is>
-          <t>selfish</t>
+          <t>farthest</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" s="1" t="inlineStr">
         <is>
-          <t>-Mr4WK0fvNb87mvQSxo3</t>
+          <t>-Mr4Ud8lbqJ_NmwqcuVd</t>
         </is>
       </c>
       <c r="B74" t="n">
-        <v>1.24</v>
+        <v>1.12</v>
       </c>
       <c r="C74" t="n">
-        <v>0.2</v>
+        <v>-0.2</v>
       </c>
       <c r="D74" t="n">
-        <v>1.24</v>
+        <v>1.12</v>
       </c>
       <c r="E74" t="n">
-        <v>0.45</v>
+        <v>0.05</v>
       </c>
       <c r="F74" t="inlineStr">
         <is>
@@ -2215,20 +2215,20 @@
     <row r="75">
       <c r="A75" s="1" t="inlineStr">
         <is>
-          <t>-Mr4WaZpBKg8-qRuOdDd</t>
+          <t>-Mr4Ui9eqdOI8EHzVilQ</t>
         </is>
       </c>
       <c r="B75" t="n">
-        <v>1.05</v>
+        <v>0.45</v>
       </c>
       <c r="C75" t="n">
-        <v>0.9999999999999999</v>
+        <v>0.5</v>
       </c>
       <c r="D75" t="n">
-        <v>1.15</v>
+        <v>0.6</v>
       </c>
       <c r="E75" t="n">
-        <v>1.15</v>
+        <v>0.6</v>
       </c>
       <c r="F75" t="inlineStr">
         <is>
@@ -2239,223 +2239,223 @@
     <row r="76">
       <c r="A76" s="1" t="inlineStr">
         <is>
-          <t>-Mr4WrJIvqPmFu6h_MeF</t>
+          <t>-Mr4UjxGLiaOpLnJm4Ij</t>
         </is>
       </c>
       <c r="B76" t="n">
-        <v>0.45</v>
+        <v>1.05</v>
       </c>
       <c r="C76" t="n">
-        <v>0.45</v>
+        <v>0.9999999999999999</v>
       </c>
       <c r="D76" t="n">
-        <v>0.5</v>
+        <v>1.15</v>
       </c>
       <c r="E76" t="n">
-        <v>0.65</v>
+        <v>1.15</v>
       </c>
       <c r="F76" t="inlineStr">
         <is>
-          <t>farthest</t>
+          <t>TSP</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" s="1" t="inlineStr">
         <is>
-          <t>-Mr4X1dmdxBYdbK5v6dD</t>
+          <t>-Mr4Ul5ReQVB0WgIXerb</t>
         </is>
       </c>
       <c r="B77" t="n">
-        <v>1.22</v>
+        <v>0.35</v>
       </c>
       <c r="C77" t="n">
-        <v>0.09999999999999998</v>
+        <v>0.4</v>
       </c>
       <c r="D77" t="n">
-        <v>1.22</v>
+        <v>0.45</v>
       </c>
       <c r="E77" t="n">
-        <v>0.35</v>
+        <v>0.55</v>
       </c>
       <c r="F77" t="inlineStr">
         <is>
-          <t>selfish</t>
+          <t>farthest</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" s="1" t="inlineStr">
         <is>
-          <t>-Mr4XDqBsRDAqHLPsq4a</t>
+          <t>-Mr4Ut1L-oObBWTyF2pw</t>
         </is>
       </c>
       <c r="B78" t="n">
-        <v>0.07000000000000001</v>
+        <v>0.6</v>
       </c>
       <c r="C78" t="n">
-        <v>0.09999999999999998</v>
+        <v>0.65</v>
       </c>
       <c r="D78" t="n">
-        <v>0.07000000000000001</v>
+        <v>0.75</v>
       </c>
       <c r="E78" t="n">
-        <v>0.35</v>
+        <v>0.75</v>
       </c>
       <c r="F78" t="inlineStr">
         <is>
-          <t>random</t>
+          <t>closest</t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" s="1" t="inlineStr">
         <is>
-          <t>-Mr4XE6mKKCDMgPxEQih</t>
+          <t>-Mr4UxBWfTjUOaulxxos</t>
         </is>
       </c>
       <c r="B79" t="n">
-        <v>1.25</v>
+        <v>0.4</v>
       </c>
       <c r="C79" t="n">
-        <v>0.25</v>
+        <v>0.35</v>
       </c>
       <c r="D79" t="n">
-        <v>1.25</v>
+        <v>0.45</v>
       </c>
       <c r="E79" t="n">
-        <v>0.5</v>
+        <v>0.55</v>
       </c>
       <c r="F79" t="inlineStr">
         <is>
-          <t>selfish</t>
+          <t>farthest</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" s="1" t="inlineStr">
         <is>
-          <t>-Mr4XETyzEOgnO1j22yP</t>
+          <t>-Mr4UxN0e26HH3gDWNqU</t>
         </is>
       </c>
       <c r="B80" t="n">
-        <v>0.7000000000000001</v>
+        <v>0.55</v>
       </c>
       <c r="C80" t="n">
-        <v>0.7</v>
+        <v>0.15</v>
       </c>
       <c r="D80" t="n">
-        <v>0.8</v>
+        <v>0.55</v>
       </c>
       <c r="E80" t="n">
-        <v>0.85</v>
+        <v>0.4</v>
       </c>
       <c r="F80" t="inlineStr">
         <is>
-          <t>closest</t>
+          <t>random</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" s="1" t="inlineStr">
         <is>
-          <t>-Mr4XJkvwu_g40rP9Eo8</t>
+          <t>-Mr4V-Ycz9bzduYJ4sQ-</t>
         </is>
       </c>
       <c r="B81" t="n">
-        <v>-1.32</v>
+        <v>0.4500000000000001</v>
       </c>
       <c r="C81" t="n">
-        <v>-0.32</v>
+        <v>0.5</v>
       </c>
       <c r="D81" t="n">
-        <v>-1.32</v>
+        <v>0.55</v>
       </c>
       <c r="E81" t="n">
-        <v>-0.07000000000000001</v>
+        <v>0.65</v>
       </c>
       <c r="F81" t="inlineStr">
         <is>
-          <t>random</t>
+          <t>farthest</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" s="1" t="inlineStr">
         <is>
-          <t>-Mr4XPad2ah2sPCiZBbQ</t>
+          <t>-Mr4V1oYgPPN0wIVmLpB</t>
         </is>
       </c>
       <c r="B82" t="n">
-        <v>0.62</v>
+        <v>0.85</v>
       </c>
       <c r="C82" t="n">
-        <v>0.3</v>
+        <v>0.7999999999999999</v>
       </c>
       <c r="D82" t="n">
-        <v>0.62</v>
+        <v>0.95</v>
       </c>
       <c r="E82" t="n">
-        <v>0.55</v>
+        <v>0.95</v>
       </c>
       <c r="F82" t="inlineStr">
         <is>
-          <t>random</t>
+          <t>TSP</t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" s="1" t="inlineStr">
         <is>
-          <t>-Mr4Xarq6jGMbIL9hqPj</t>
+          <t>-Mr4V2R-FuAlrB31ccSL</t>
         </is>
       </c>
       <c r="B83" t="n">
-        <v>-2.1</v>
+        <v>0.5499999999999999</v>
       </c>
       <c r="C83" t="n">
-        <v>-0.5</v>
+        <v>0.59</v>
       </c>
       <c r="D83" t="n">
-        <v>-2.05</v>
+        <v>0.7</v>
       </c>
       <c r="E83" t="n">
-        <v>-0.3</v>
+        <v>0.6899999999999999</v>
       </c>
       <c r="F83" t="inlineStr">
         <is>
-          <t>random</t>
+          <t>closest</t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="A84" s="1" t="inlineStr">
         <is>
-          <t>-Mr4XwqTEFWFg-74Phzt</t>
+          <t>-Mr4VCw2qL_Bo6gK2Gde</t>
         </is>
       </c>
       <c r="B84" t="n">
-        <v>0.28</v>
+        <v>0.75</v>
       </c>
       <c r="C84" t="n">
-        <v>0</v>
+        <v>0.7</v>
       </c>
       <c r="D84" t="n">
-        <v>0.28</v>
+        <v>0.85</v>
       </c>
       <c r="E84" t="n">
-        <v>0.25</v>
+        <v>0.85</v>
       </c>
       <c r="F84" t="inlineStr">
         <is>
-          <t>random</t>
+          <t>closest</t>
         </is>
       </c>
     </row>
     <row r="85">
       <c r="A85" s="1" t="inlineStr">
         <is>
-          <t>-Mr4YGELjDJsbJF3JXQ-</t>
+          <t>-Mr4VDiaPe3ffgXJITBM</t>
         </is>
       </c>
       <c r="B85" t="n">
@@ -2479,20 +2479,20 @@
     <row r="86">
       <c r="A86" s="1" t="inlineStr">
         <is>
-          <t>-Mr4YU2QdskQ9MHXGYx0</t>
+          <t>-Mr4VHIAFIXo8DhoUVKp</t>
         </is>
       </c>
       <c r="B86" t="n">
-        <v>0.75</v>
+        <v>0.45</v>
       </c>
       <c r="C86" t="n">
-        <v>0.7</v>
+        <v>0.77</v>
       </c>
       <c r="D86" t="n">
-        <v>0.85</v>
+        <v>0.6</v>
       </c>
       <c r="E86" t="n">
-        <v>0.85</v>
+        <v>0.87</v>
       </c>
       <c r="F86" t="inlineStr">
         <is>
@@ -2503,20 +2503,20 @@
     <row r="87">
       <c r="A87" s="1" t="inlineStr">
         <is>
-          <t>-Mr4YUSiJELSIibuYZ-C</t>
+          <t>-Mr4VKFfLDB45xOtua-M</t>
         </is>
       </c>
       <c r="B87" t="n">
-        <v>0.45</v>
+        <v>0.86</v>
       </c>
       <c r="C87" t="n">
-        <v>0.45</v>
+        <v>0.09999999999999998</v>
       </c>
       <c r="D87" t="n">
-        <v>0.5</v>
+        <v>0.96</v>
       </c>
       <c r="E87" t="n">
-        <v>0.65</v>
+        <v>0.25</v>
       </c>
       <c r="F87" t="inlineStr">
         <is>
@@ -2527,92 +2527,92 @@
     <row r="88">
       <c r="A88" s="1" t="inlineStr">
         <is>
-          <t>-Mr4YYprkXmy_Tw3G2LD</t>
+          <t>-Mr4VKfA5qbbsqbEFQ9B</t>
         </is>
       </c>
       <c r="B88" t="n">
-        <v>0.48</v>
+        <v>0.65</v>
       </c>
       <c r="C88" t="n">
-        <v>0.2</v>
+        <v>0.7</v>
       </c>
       <c r="D88" t="n">
-        <v>0.48</v>
+        <v>0.75</v>
       </c>
       <c r="E88" t="n">
-        <v>0.45</v>
+        <v>0.85</v>
       </c>
       <c r="F88" t="inlineStr">
         <is>
-          <t>random</t>
+          <t>closest</t>
         </is>
       </c>
     </row>
     <row r="89">
       <c r="A89" s="1" t="inlineStr">
         <is>
-          <t>-Mr4YeTN_rlR_jYTeeo8</t>
+          <t>-Mr4VRV9hRV-yTio4Z7s</t>
         </is>
       </c>
       <c r="B89" t="n">
-        <v>0.85</v>
+        <v>1.12</v>
       </c>
       <c r="C89" t="n">
-        <v>0.85</v>
+        <v>-0.3</v>
       </c>
       <c r="D89" t="n">
-        <v>1</v>
+        <v>1.12</v>
       </c>
       <c r="E89" t="n">
-        <v>0.95</v>
+        <v>-0.05</v>
       </c>
       <c r="F89" t="inlineStr">
         <is>
-          <t>closest</t>
+          <t>selfish</t>
         </is>
       </c>
     </row>
     <row r="90">
       <c r="A90" s="1" t="inlineStr">
         <is>
-          <t>-Mr4YenZ3l1KqpIlPwax</t>
+          <t>-Mr4VSwtCpefFtvQrTEX</t>
         </is>
       </c>
       <c r="B90" t="n">
-        <v>1.05</v>
+        <v>1.24</v>
       </c>
       <c r="C90" t="n">
-        <v>0.9999999999999999</v>
+        <v>0.3</v>
       </c>
       <c r="D90" t="n">
-        <v>1.15</v>
+        <v>1.24</v>
       </c>
       <c r="E90" t="n">
-        <v>1.15</v>
+        <v>0.55</v>
       </c>
       <c r="F90" t="inlineStr">
         <is>
-          <t>TSP</t>
+          <t>selfish</t>
         </is>
       </c>
     </row>
     <row r="91">
       <c r="A91" s="1" t="inlineStr">
         <is>
-          <t>-Mr4Yrtg2Rk8u83xa6yl</t>
+          <t>-Mr4VrgeSScBxw-VOkCj</t>
         </is>
       </c>
       <c r="B91" t="n">
-        <v>1.04</v>
+        <v>1.26</v>
       </c>
       <c r="C91" t="n">
-        <v>-0.5700000000000001</v>
+        <v>0.3</v>
       </c>
       <c r="D91" t="n">
-        <v>1.04</v>
+        <v>1.26</v>
       </c>
       <c r="E91" t="n">
-        <v>-0.32</v>
+        <v>0.55</v>
       </c>
       <c r="F91" t="inlineStr">
         <is>
@@ -2623,188 +2623,188 @@
     <row r="92">
       <c r="A92" s="1" t="inlineStr">
         <is>
-          <t>-Mr4Z-X5zg1KsbiluQuS</t>
+          <t>-Mr4VvMxhAb1yIPOQ0tV</t>
         </is>
       </c>
       <c r="B92" t="n">
-        <v>1.25</v>
+        <v>0.71</v>
       </c>
       <c r="C92" t="n">
-        <v>0.29</v>
+        <v>0.35</v>
       </c>
       <c r="D92" t="n">
-        <v>1.25</v>
+        <v>0.76</v>
       </c>
       <c r="E92" t="n">
-        <v>0.54</v>
+        <v>0.55</v>
       </c>
       <c r="F92" t="inlineStr">
         <is>
-          <t>selfish</t>
+          <t>random</t>
         </is>
       </c>
     </row>
     <row r="93">
       <c r="A93" s="1" t="inlineStr">
         <is>
-          <t>-Mr4Z4HKOdKtiLTbH1_T</t>
+          <t>-Mr4VyzMcKi-TVbEWVbs</t>
         </is>
       </c>
       <c r="B93" t="n">
-        <v>1.05</v>
+        <v>-0.3</v>
       </c>
       <c r="C93" t="n">
-        <v>0.9999999999999999</v>
+        <v>0.22</v>
       </c>
       <c r="D93" t="n">
-        <v>1.15</v>
+        <v>-0.25</v>
       </c>
       <c r="E93" t="n">
-        <v>1.15</v>
+        <v>0.42</v>
       </c>
       <c r="F93" t="inlineStr">
         <is>
-          <t>TSP</t>
+          <t>farthest</t>
         </is>
       </c>
     </row>
     <row r="94">
       <c r="A94" s="1" t="inlineStr">
         <is>
-          <t>-Mr4Z8rUbHdUZs5MlX5L</t>
+          <t>-Mr4Vzctm_Axuz_zPELo</t>
         </is>
       </c>
       <c r="B94" t="n">
-        <v>0.75</v>
+        <v>0.35</v>
       </c>
       <c r="C94" t="n">
-        <v>0.7</v>
+        <v>0.35</v>
       </c>
       <c r="D94" t="n">
-        <v>0.85</v>
+        <v>0.45</v>
       </c>
       <c r="E94" t="n">
-        <v>0.85</v>
+        <v>0.5</v>
       </c>
       <c r="F94" t="inlineStr">
         <is>
-          <t>closest</t>
+          <t>farthest</t>
         </is>
       </c>
     </row>
     <row r="95">
       <c r="A95" s="1" t="inlineStr">
         <is>
-          <t>-Mr4ZDUjNRhhhb3waqx3</t>
+          <t>-Mr4W4EWZ2YgC3PURuQT</t>
         </is>
       </c>
       <c r="B95" t="n">
-        <v>0.63</v>
+        <v>0.15</v>
       </c>
       <c r="C95" t="n">
-        <v>0.3</v>
+        <v>0.35</v>
       </c>
       <c r="D95" t="n">
-        <v>0.63</v>
+        <v>0.2</v>
       </c>
       <c r="E95" t="n">
         <v>0.55</v>
       </c>
       <c r="F95" t="inlineStr">
         <is>
-          <t>random</t>
+          <t>farthest</t>
         </is>
       </c>
     </row>
     <row r="96">
       <c r="A96" s="1" t="inlineStr">
         <is>
-          <t>-Mr4ZFMnT2YnhWH5wQMr</t>
+          <t>-Mr4WEHdyw5TmHtu1p8h</t>
         </is>
       </c>
       <c r="B96" t="n">
-        <v>0.4</v>
+        <v>0.91</v>
       </c>
       <c r="C96" t="n">
-        <v>0.4399999999999999</v>
+        <v>-0.04999999999999999</v>
       </c>
       <c r="D96" t="n">
-        <v>0.5</v>
+        <v>0.91</v>
       </c>
       <c r="E96" t="n">
-        <v>0.59</v>
+        <v>0.2</v>
       </c>
       <c r="F96" t="inlineStr">
         <is>
-          <t>closest</t>
+          <t>selfish</t>
         </is>
       </c>
     </row>
     <row r="97">
       <c r="A97" s="1" t="inlineStr">
         <is>
-          <t>-Mr4ZKxk_F3bcL0G6hYB</t>
+          <t>-Mr4WK0fvNb87mvQSxo3</t>
         </is>
       </c>
       <c r="B97" t="n">
-        <v>0.51</v>
+        <v>1.24</v>
       </c>
       <c r="C97" t="n">
-        <v>0.15</v>
+        <v>0.2</v>
       </c>
       <c r="D97" t="n">
-        <v>0.51</v>
+        <v>1.24</v>
       </c>
       <c r="E97" t="n">
-        <v>0.4</v>
+        <v>0.45</v>
       </c>
       <c r="F97" t="inlineStr">
         <is>
-          <t>random</t>
+          <t>selfish</t>
         </is>
       </c>
     </row>
     <row r="98">
       <c r="A98" s="1" t="inlineStr">
         <is>
-          <t>-Mr4ZLOkU0-yjZv7Ue6e</t>
+          <t>-Mr4WMaCGVrAaemGSs3h</t>
         </is>
       </c>
       <c r="B98" t="n">
-        <v>-0.5800000000000001</v>
+        <v>1.17</v>
       </c>
       <c r="C98" t="n">
-        <v>-1.1</v>
+        <v>-0.11</v>
       </c>
       <c r="D98" t="n">
-        <v>-0.53</v>
+        <v>1.17</v>
       </c>
       <c r="E98" t="n">
-        <v>-0.9</v>
+        <v>0.14</v>
       </c>
       <c r="F98" t="inlineStr">
         <is>
-          <t>random</t>
+          <t>selfish</t>
         </is>
       </c>
     </row>
     <row r="99">
       <c r="A99" s="1" t="inlineStr">
         <is>
-          <t>-Mr4ZP1uRZQOMbSo7-rN</t>
+          <t>-Mr4WaZpBKg8-qRuOdDd</t>
         </is>
       </c>
       <c r="B99" t="n">
-        <v>0.25</v>
+        <v>1.05</v>
       </c>
       <c r="C99" t="n">
-        <v>0.3</v>
+        <v>0.9999999999999999</v>
       </c>
       <c r="D99" t="n">
-        <v>0.5</v>
+        <v>1.15</v>
       </c>
       <c r="E99" t="n">
-        <v>0.3</v>
+        <v>1.15</v>
       </c>
       <c r="F99" t="inlineStr">
         <is>
@@ -2815,68 +2815,68 @@
     <row r="100">
       <c r="A100" s="1" t="inlineStr">
         <is>
-          <t>-Mr4ZSnoXZPveZc7ldl3</t>
+          <t>-Mr4WoMyn495McY7Kzei</t>
         </is>
       </c>
       <c r="B100" t="n">
-        <v>1.1</v>
+        <v>0.7000000000000001</v>
       </c>
       <c r="C100" t="n">
-        <v>-0.04999999999999999</v>
+        <v>0.65</v>
       </c>
       <c r="D100" t="n">
-        <v>1.1</v>
+        <v>0.8</v>
       </c>
       <c r="E100" t="n">
-        <v>0.2</v>
+        <v>0.8</v>
       </c>
       <c r="F100" t="inlineStr">
         <is>
-          <t>selfish</t>
+          <t>closest</t>
         </is>
       </c>
     </row>
     <row r="101">
       <c r="A101" s="1" t="inlineStr">
         <is>
-          <t>-Mr4ZWSrgCzM3TlhrUpA</t>
+          <t>-Mr4WrJIvqPmFu6h_MeF</t>
         </is>
       </c>
       <c r="B101" t="n">
-        <v>0.25</v>
+        <v>0.45</v>
       </c>
       <c r="C101" t="n">
-        <v>0.97</v>
+        <v>0.45</v>
       </c>
       <c r="D101" t="n">
         <v>0.5</v>
       </c>
       <c r="E101" t="n">
-        <v>1.02</v>
+        <v>0.65</v>
       </c>
       <c r="F101" t="inlineStr">
         <is>
-          <t>TSP</t>
+          <t>farthest</t>
         </is>
       </c>
     </row>
     <row r="102">
       <c r="A102" s="1" t="inlineStr">
         <is>
-          <t>-Mr4ZZD8-_T-ITkFbNu1</t>
+          <t>-Mr4X1dmdxBYdbK5v6dD</t>
         </is>
       </c>
       <c r="B102" t="n">
-        <v>1.19</v>
+        <v>1.22</v>
       </c>
       <c r="C102" t="n">
-        <v>0.07000000000000001</v>
+        <v>0.09999999999999998</v>
       </c>
       <c r="D102" t="n">
-        <v>1.19</v>
+        <v>1.22</v>
       </c>
       <c r="E102" t="n">
-        <v>0.32</v>
+        <v>0.35</v>
       </c>
       <c r="F102" t="inlineStr">
         <is>
@@ -2887,20 +2887,20 @@
     <row r="103">
       <c r="A103" s="1" t="inlineStr">
         <is>
-          <t>-Mr4Zv2TnMWi8pXYaSPy</t>
+          <t>-Mr4XDqBsRDAqHLPsq4a</t>
         </is>
       </c>
       <c r="B103" t="n">
-        <v>0.03</v>
+        <v>0.07000000000000001</v>
       </c>
       <c r="C103" t="n">
-        <v>-0.04999999999999999</v>
+        <v>0.09999999999999998</v>
       </c>
       <c r="D103" t="n">
-        <v>0.03</v>
+        <v>0.07000000000000001</v>
       </c>
       <c r="E103" t="n">
-        <v>0.2</v>
+        <v>0.35</v>
       </c>
       <c r="F103" t="inlineStr">
         <is>
@@ -2911,188 +2911,188 @@
     <row r="104">
       <c r="A104" s="1" t="inlineStr">
         <is>
-          <t>-Mr4Zw08vxDeIWifKmcp</t>
+          <t>-Mr4XE6mKKCDMgPxEQih</t>
         </is>
       </c>
       <c r="B104" t="n">
-        <v>0.4</v>
+        <v>1.25</v>
       </c>
       <c r="C104" t="n">
-        <v>0.4500000000000001</v>
+        <v>0.25</v>
       </c>
       <c r="D104" t="n">
-        <v>0.55</v>
+        <v>1.25</v>
       </c>
       <c r="E104" t="n">
-        <v>0.55</v>
+        <v>0.5</v>
       </c>
       <c r="F104" t="inlineStr">
         <is>
-          <t>farthest</t>
+          <t>selfish</t>
         </is>
       </c>
     </row>
     <row r="105">
       <c r="A105" s="1" t="inlineStr">
         <is>
-          <t>-Mr4_ICrbKPcl3Cztxwb</t>
+          <t>-Mr4XETyzEOgnO1j22yP</t>
         </is>
       </c>
       <c r="B105" t="n">
-        <v>0.33</v>
+        <v>0.7000000000000001</v>
       </c>
       <c r="C105" t="n">
-        <v>0.57</v>
+        <v>0.7</v>
       </c>
       <c r="D105" t="n">
-        <v>0.43</v>
+        <v>0.8</v>
       </c>
       <c r="E105" t="n">
-        <v>0.72</v>
+        <v>0.85</v>
       </c>
       <c r="F105" t="inlineStr">
         <is>
-          <t>random</t>
+          <t>closest</t>
         </is>
       </c>
     </row>
     <row r="106">
       <c r="A106" s="1" t="inlineStr">
         <is>
-          <t>-Mr4_c1eWQi5mALBc8Vb</t>
+          <t>-Mr4XIuf6_45lcNJuU12</t>
         </is>
       </c>
       <c r="B106" t="n">
-        <v>-0.18</v>
+        <v>0.5</v>
       </c>
       <c r="C106" t="n">
-        <v>-0.01999999999999999</v>
+        <v>0.45</v>
       </c>
       <c r="D106" t="n">
-        <v>-0.18</v>
+        <v>0.55</v>
       </c>
       <c r="E106" t="n">
-        <v>0.23</v>
+        <v>0.65</v>
       </c>
       <c r="F106" t="inlineStr">
         <is>
-          <t>random</t>
+          <t>farthest</t>
         </is>
       </c>
     </row>
     <row r="107">
       <c r="A107" s="1" t="inlineStr">
         <is>
-          <t>-Mr4bNQJo1l3U7zrP2PJ</t>
+          <t>-Mr4XJkvwu_g40rP9Eo8</t>
         </is>
       </c>
       <c r="B107" t="n">
-        <v>-1.34</v>
+        <v>-1.32</v>
       </c>
       <c r="C107" t="n">
-        <v>-1.5</v>
+        <v>-0.32</v>
       </c>
       <c r="D107" t="n">
-        <v>-1.24</v>
+        <v>-1.32</v>
       </c>
       <c r="E107" t="n">
-        <v>-1.35</v>
+        <v>-0.07000000000000001</v>
       </c>
       <c r="F107" t="inlineStr">
         <is>
-          <t>farthest</t>
+          <t>random</t>
         </is>
       </c>
     </row>
     <row r="108">
       <c r="A108" s="1" t="inlineStr">
         <is>
-          <t>-Mr4bWLBRG3475BpxIUJ</t>
+          <t>-Mr4XPad2ah2sPCiZBbQ</t>
         </is>
       </c>
       <c r="B108" t="n">
-        <v>0.7000000000000001</v>
+        <v>0.62</v>
       </c>
       <c r="C108" t="n">
-        <v>0.7</v>
+        <v>0.3</v>
       </c>
       <c r="D108" t="n">
-        <v>0.8</v>
+        <v>0.62</v>
       </c>
       <c r="E108" t="n">
-        <v>0.85</v>
+        <v>0.55</v>
       </c>
       <c r="F108" t="inlineStr">
         <is>
-          <t>closest</t>
+          <t>random</t>
         </is>
       </c>
     </row>
     <row r="109">
       <c r="A109" s="1" t="inlineStr">
         <is>
-          <t>-Mr4bY4JZ3gTh04PmI0D</t>
+          <t>-Mr4Xarq6jGMbIL9hqPj</t>
         </is>
       </c>
       <c r="B109" t="n">
-        <v>1</v>
+        <v>-2.1</v>
       </c>
       <c r="C109" t="n">
-        <v>0.9999999999999999</v>
+        <v>-0.5</v>
       </c>
       <c r="D109" t="n">
-        <v>1.1</v>
+        <v>-2.05</v>
       </c>
       <c r="E109" t="n">
-        <v>1.15</v>
+        <v>-0.3</v>
       </c>
       <c r="F109" t="inlineStr">
         <is>
-          <t>TSP</t>
+          <t>random</t>
         </is>
       </c>
     </row>
     <row r="110">
       <c r="A110" s="1" t="inlineStr">
         <is>
-          <t>-Mr4d6kLpnPruwzbNjeh</t>
+          <t>-Mr4XwqTEFWFg-74Phzt</t>
         </is>
       </c>
       <c r="B110" t="n">
-        <v>1.26</v>
+        <v>0.28</v>
       </c>
       <c r="C110" t="n">
-        <v>0.3</v>
+        <v>0</v>
       </c>
       <c r="D110" t="n">
-        <v>1.26</v>
+        <v>0.28</v>
       </c>
       <c r="E110" t="n">
-        <v>0.55</v>
+        <v>0.25</v>
       </c>
       <c r="F110" t="inlineStr">
         <is>
-          <t>selfish</t>
+          <t>random</t>
         </is>
       </c>
     </row>
     <row r="111">
       <c r="A111" s="1" t="inlineStr">
         <is>
-          <t>-Mr4eWG-5xqB9Q6Dnmv3</t>
+          <t>-Mr4YB4Gs4MBk_2-XPG5</t>
         </is>
       </c>
       <c r="B111" t="n">
-        <v>0.5499999999999999</v>
+        <v>0.85</v>
       </c>
       <c r="C111" t="n">
-        <v>0.79</v>
+        <v>0.7</v>
       </c>
       <c r="D111" t="n">
-        <v>0.7</v>
+        <v>0.95</v>
       </c>
       <c r="E111" t="n">
-        <v>0.89</v>
+        <v>0.85</v>
       </c>
       <c r="F111" t="inlineStr">
         <is>
@@ -3103,44 +3103,44 @@
     <row r="112">
       <c r="A112" s="1" t="inlineStr">
         <is>
-          <t>-Mr4ej5yR8BD_KnrALKV</t>
+          <t>-Mr4YGELjDJsbJF3JXQ-</t>
         </is>
       </c>
       <c r="B112" t="n">
-        <v>0.29</v>
+        <v>1.05</v>
       </c>
       <c r="C112" t="n">
-        <v>0.29</v>
+        <v>0.9999999999999999</v>
       </c>
       <c r="D112" t="n">
-        <v>0.39</v>
+        <v>1.15</v>
       </c>
       <c r="E112" t="n">
-        <v>0.44</v>
+        <v>1.15</v>
       </c>
       <c r="F112" t="inlineStr">
         <is>
-          <t>random</t>
+          <t>TSP</t>
         </is>
       </c>
     </row>
     <row r="113">
       <c r="A113" s="1" t="inlineStr">
         <is>
-          <t>-Mr4eseUbQr_kkfGoJiA</t>
+          <t>-Mr4YU2QdskQ9MHXGYx0</t>
         </is>
       </c>
       <c r="B113" t="n">
-        <v>0.7000000000000001</v>
+        <v>0.75</v>
       </c>
       <c r="C113" t="n">
-        <v>0.6899999999999999</v>
+        <v>0.7</v>
       </c>
       <c r="D113" t="n">
-        <v>0.8</v>
+        <v>0.85</v>
       </c>
       <c r="E113" t="n">
-        <v>0.84</v>
+        <v>0.85</v>
       </c>
       <c r="F113" t="inlineStr">
         <is>
@@ -3151,68 +3151,68 @@
     <row r="114">
       <c r="A114" s="1" t="inlineStr">
         <is>
-          <t>-Mr4et1M31FSgHYxaXto</t>
+          <t>-Mr4YUSiJELSIibuYZ-C</t>
         </is>
       </c>
       <c r="B114" t="n">
-        <v>0.66</v>
+        <v>0.45</v>
       </c>
       <c r="C114" t="n">
-        <v>0.3</v>
+        <v>0.45</v>
       </c>
       <c r="D114" t="n">
-        <v>0.66</v>
+        <v>0.5</v>
       </c>
       <c r="E114" t="n">
-        <v>0.55</v>
+        <v>0.65</v>
       </c>
       <c r="F114" t="inlineStr">
         <is>
-          <t>random</t>
+          <t>farthest</t>
         </is>
       </c>
     </row>
     <row r="115">
       <c r="A115" s="1" t="inlineStr">
         <is>
-          <t>-Mr4eyZJx-gU5Cacgqq-</t>
+          <t>-Mr4YYprkXmy_Tw3G2LD</t>
         </is>
       </c>
       <c r="B115" t="n">
-        <v>0.9500000000000001</v>
+        <v>0.48</v>
       </c>
       <c r="C115" t="n">
-        <v>0.9500000000000001</v>
+        <v>0.2</v>
       </c>
       <c r="D115" t="n">
-        <v>1.05</v>
+        <v>0.48</v>
       </c>
       <c r="E115" t="n">
-        <v>1.1</v>
+        <v>0.45</v>
       </c>
       <c r="F115" t="inlineStr">
         <is>
-          <t>TSP</t>
+          <t>random</t>
         </is>
       </c>
     </row>
     <row r="116">
       <c r="A116" s="1" t="inlineStr">
         <is>
-          <t>-Mr4f3EUA-I93xEt4s-W</t>
+          <t>-Mr4YeTN_rlR_jYTeeo8</t>
         </is>
       </c>
       <c r="B116" t="n">
-        <v>0.8</v>
+        <v>0.85</v>
       </c>
       <c r="C116" t="n">
-        <v>0.7</v>
+        <v>0.85</v>
       </c>
       <c r="D116" t="n">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="E116" t="n">
-        <v>0.85</v>
+        <v>0.95</v>
       </c>
       <c r="F116" t="inlineStr">
         <is>
@@ -3223,113 +3223,113 @@
     <row r="117">
       <c r="A117" s="1" t="inlineStr">
         <is>
-          <t>-Mr4f4NUS_ANE-GljaXl</t>
+          <t>-Mr4YenZ3l1KqpIlPwax</t>
         </is>
       </c>
       <c r="B117" t="n">
-        <v>0.55</v>
+        <v>1.05</v>
       </c>
       <c r="C117" t="n">
-        <v>0.5</v>
+        <v>0.9999999999999999</v>
       </c>
       <c r="D117" t="n">
-        <v>0.65</v>
+        <v>1.15</v>
       </c>
       <c r="E117" t="n">
-        <v>0.65</v>
+        <v>1.15</v>
       </c>
       <c r="F117" t="inlineStr">
         <is>
-          <t>closest</t>
+          <t>TSP</t>
         </is>
       </c>
     </row>
     <row r="118">
       <c r="A118" s="1" t="inlineStr">
         <is>
-          <t>-Mr4fBZl_62qSc_4RnDv</t>
+          <t>-Mr4Yrtg2Rk8u83xa6yl</t>
         </is>
       </c>
       <c r="B118" t="n">
-        <v>1</v>
+        <v>1.04</v>
       </c>
       <c r="C118" t="n">
-        <v>0.9999999999999999</v>
+        <v>-0.5700000000000001</v>
       </c>
       <c r="D118" t="n">
-        <v>1.1</v>
+        <v>1.04</v>
       </c>
       <c r="E118" t="n">
-        <v>1.15</v>
+        <v>-0.32</v>
       </c>
       <c r="F118" t="inlineStr">
         <is>
-          <t>TSP</t>
+          <t>selfish</t>
         </is>
       </c>
     </row>
     <row r="119">
       <c r="A119" s="1" t="inlineStr">
         <is>
-          <t>-Mr4fC9EkjHHPnr1zUd8</t>
+          <t>-Mr4Ywb1g26lheX10uAu</t>
         </is>
       </c>
       <c r="B119" t="n">
-        <v>0.65</v>
+        <v>1</v>
       </c>
       <c r="C119" t="n">
-        <v>0.6</v>
+        <v>0.9999999999999999</v>
       </c>
       <c r="D119" t="n">
-        <v>0.75</v>
+        <v>1.1</v>
       </c>
       <c r="E119" t="n">
-        <v>0.75</v>
+        <v>1.15</v>
       </c>
       <c r="F119" t="inlineStr">
         <is>
-          <t>closest</t>
+          <t>TSP</t>
         </is>
       </c>
     </row>
     <row r="120">
       <c r="A120" s="1" t="inlineStr">
         <is>
-          <t>-Mr4fa-QIY2yVwGZExoD</t>
+          <t>-Mr4Z-X5zg1KsbiluQuS</t>
         </is>
       </c>
       <c r="B120" t="n">
-        <v>0.25</v>
+        <v>1.25</v>
       </c>
       <c r="C120" t="n">
-        <v>0.25</v>
+        <v>0.29</v>
       </c>
       <c r="D120" t="n">
-        <v>0.25</v>
+        <v>1.25</v>
       </c>
       <c r="E120" t="n">
-        <v>0.5</v>
+        <v>0.54</v>
       </c>
       <c r="F120" t="inlineStr">
         <is>
-          <t>random</t>
+          <t>selfish</t>
         </is>
       </c>
     </row>
     <row r="121">
       <c r="A121" s="1" t="inlineStr">
         <is>
-          <t>-Mr4ffBo8AxSYU6oNxDV</t>
+          <t>-Mr4Z4HKOdKtiLTbH1_T</t>
         </is>
       </c>
       <c r="B121" t="n">
-        <v>1</v>
+        <v>1.05</v>
       </c>
       <c r="C121" t="n">
         <v>0.9999999999999999</v>
       </c>
       <c r="D121" t="n">
-        <v>1.1</v>
+        <v>1.15</v>
       </c>
       <c r="E121" t="n">
         <v>1.15</v>
@@ -3343,236 +3343,236 @@
     <row r="122">
       <c r="A122" s="1" t="inlineStr">
         <is>
-          <t>-Mr4fiUqvTaGet47n6rF</t>
+          <t>-Mr4Z8rUbHdUZs5MlX5L</t>
         </is>
       </c>
       <c r="B122" t="n">
-        <v>1.05</v>
+        <v>0.75</v>
       </c>
       <c r="C122" t="n">
-        <v>0.9999999999999999</v>
+        <v>0.7</v>
       </c>
       <c r="D122" t="n">
-        <v>1.15</v>
+        <v>0.85</v>
       </c>
       <c r="E122" t="n">
-        <v>1.15</v>
+        <v>0.85</v>
       </c>
       <c r="F122" t="inlineStr">
         <is>
-          <t>TSP</t>
+          <t>closest</t>
         </is>
       </c>
     </row>
     <row r="123">
       <c r="A123" s="1" t="inlineStr">
         <is>
-          <t>-Mr4gAjnlvcW3RKZX703</t>
+          <t>-Mr4ZAu7n2mO5sYZwfsM</t>
         </is>
       </c>
       <c r="B123" t="n">
-        <v>0.15</v>
+        <v>0.63</v>
       </c>
       <c r="C123" t="n">
-        <v>1.19</v>
+        <v>0.3</v>
       </c>
       <c r="D123" t="n">
-        <v>0.4</v>
+        <v>0.63</v>
       </c>
       <c r="E123" t="n">
-        <v>1.24</v>
+        <v>0.55</v>
       </c>
       <c r="F123" t="inlineStr">
         <is>
-          <t>closest</t>
+          <t>random</t>
         </is>
       </c>
     </row>
     <row r="124">
       <c r="A124" s="1" t="inlineStr">
         <is>
-          <t>-Mr4gIM5ATsxVHYlUnPm</t>
+          <t>-Mr4ZDUjNRhhhb3waqx3</t>
         </is>
       </c>
       <c r="B124" t="n">
-        <v>1.22</v>
+        <v>0.63</v>
       </c>
       <c r="C124" t="n">
-        <v>0.22</v>
+        <v>0.3</v>
       </c>
       <c r="D124" t="n">
-        <v>1.22</v>
+        <v>0.63</v>
       </c>
       <c r="E124" t="n">
-        <v>0.47</v>
+        <v>0.55</v>
       </c>
       <c r="F124" t="inlineStr">
         <is>
-          <t>selfish</t>
+          <t>random</t>
         </is>
       </c>
     </row>
     <row r="125">
       <c r="A125" s="1" t="inlineStr">
         <is>
-          <t>-Mr4gM9iXWa0OxaNz9pd</t>
+          <t>-Mr4ZFMnT2YnhWH5wQMr</t>
         </is>
       </c>
       <c r="B125" t="n">
-        <v>1.26</v>
+        <v>0.4</v>
       </c>
       <c r="C125" t="n">
-        <v>0.35</v>
+        <v>0.4399999999999999</v>
       </c>
       <c r="D125" t="n">
-        <v>1.26</v>
+        <v>0.5</v>
       </c>
       <c r="E125" t="n">
-        <v>0.6</v>
+        <v>0.59</v>
       </c>
       <c r="F125" t="inlineStr">
         <is>
-          <t>selfish</t>
+          <t>closest</t>
         </is>
       </c>
     </row>
     <row r="126">
       <c r="A126" s="1" t="inlineStr">
         <is>
-          <t>-Mr4gnhvp8zu4hyKSHT8</t>
+          <t>-Mr4ZKxk_F3bcL0G6hYB</t>
         </is>
       </c>
       <c r="B126" t="n">
-        <v>1</v>
+        <v>0.51</v>
       </c>
       <c r="C126" t="n">
-        <v>0.9999999999999999</v>
+        <v>0.15</v>
       </c>
       <c r="D126" t="n">
-        <v>1.1</v>
+        <v>0.51</v>
       </c>
       <c r="E126" t="n">
-        <v>1.15</v>
+        <v>0.4</v>
       </c>
       <c r="F126" t="inlineStr">
         <is>
-          <t>TSP</t>
+          <t>random</t>
         </is>
       </c>
     </row>
     <row r="127">
       <c r="A127" s="1" t="inlineStr">
         <is>
-          <t>-Mr4gppr7Vw6iIfcH6fv</t>
+          <t>-Mr4ZLOkU0-yjZv7Ue6e</t>
         </is>
       </c>
       <c r="B127" t="n">
-        <v>0</v>
+        <v>-0.5800000000000001</v>
       </c>
       <c r="C127" t="n">
-        <v>0</v>
+        <v>-1.1</v>
       </c>
       <c r="D127" t="n">
-        <v>0.05</v>
+        <v>-0.53</v>
       </c>
       <c r="E127" t="n">
-        <v>0.2</v>
+        <v>-0.9</v>
       </c>
       <c r="F127" t="inlineStr">
         <is>
-          <t>farthest</t>
+          <t>random</t>
         </is>
       </c>
     </row>
     <row r="128">
       <c r="A128" s="1" t="inlineStr">
         <is>
-          <t>-Mr4grc_XL69ykWx-MHR</t>
+          <t>-Mr4ZP1uRZQOMbSo7-rN</t>
         </is>
       </c>
       <c r="B128" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="C128" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="D128" t="n">
         <v>0.5</v>
       </c>
-      <c r="C128" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="D128" t="n">
-        <v>0.65</v>
-      </c>
       <c r="E128" t="n">
-        <v>0.6</v>
+        <v>0.3</v>
       </c>
       <c r="F128" t="inlineStr">
         <is>
-          <t>closest</t>
+          <t>TSP</t>
         </is>
       </c>
     </row>
     <row r="129">
       <c r="A129" s="1" t="inlineStr">
         <is>
-          <t>-Mr4hCX2_mf23fh_HfHD</t>
+          <t>-Mr4ZSnoXZPveZc7ldl3</t>
         </is>
       </c>
       <c r="B129" t="n">
-        <v>0.65</v>
+        <v>1.1</v>
       </c>
       <c r="C129" t="n">
-        <v>0.64</v>
+        <v>-0.04999999999999999</v>
       </c>
       <c r="D129" t="n">
-        <v>0.8</v>
+        <v>1.1</v>
       </c>
       <c r="E129" t="n">
-        <v>0.74</v>
+        <v>0.2</v>
       </c>
       <c r="F129" t="inlineStr">
         <is>
-          <t>closest</t>
+          <t>selfish</t>
         </is>
       </c>
     </row>
     <row r="130">
       <c r="A130" s="1" t="inlineStr">
         <is>
-          <t>-Mr4hOoZjliyARNml8Tv</t>
+          <t>-Mr4ZTi8ocgh18TWkOxO</t>
         </is>
       </c>
       <c r="B130" t="n">
-        <v>0.45</v>
+        <v>1.1</v>
       </c>
       <c r="C130" t="n">
-        <v>0.45</v>
+        <v>0.9999999999999999</v>
       </c>
       <c r="D130" t="n">
-        <v>0.5</v>
+        <v>1.2</v>
       </c>
       <c r="E130" t="n">
-        <v>0.65</v>
+        <v>1.15</v>
       </c>
       <c r="F130" t="inlineStr">
         <is>
-          <t>farthest</t>
+          <t>TSP</t>
         </is>
       </c>
     </row>
     <row r="131">
       <c r="A131" s="1" t="inlineStr">
         <is>
-          <t>-Mr4hSrulYrbm5UIrKMF</t>
+          <t>-Mr4ZWSrgCzM3TlhrUpA</t>
         </is>
       </c>
       <c r="B131" t="n">
-        <v>0.55</v>
+        <v>0.25</v>
       </c>
       <c r="C131" t="n">
-        <v>0.71</v>
+        <v>0.97</v>
       </c>
       <c r="D131" t="n">
-        <v>0.75</v>
+        <v>0.5</v>
       </c>
       <c r="E131" t="n">
-        <v>0.76</v>
+        <v>1.02</v>
       </c>
       <c r="F131" t="inlineStr">
         <is>
@@ -3583,44 +3583,44 @@
     <row r="132">
       <c r="A132" s="1" t="inlineStr">
         <is>
-          <t>-Mr4hYkL43oy86Glh53W</t>
+          <t>-Mr4ZZD8-_T-ITkFbNu1</t>
         </is>
       </c>
       <c r="B132" t="n">
-        <v>0.5</v>
+        <v>1.19</v>
       </c>
       <c r="C132" t="n">
-        <v>0.5</v>
+        <v>0.07000000000000001</v>
       </c>
       <c r="D132" t="n">
-        <v>0.65</v>
+        <v>1.19</v>
       </c>
       <c r="E132" t="n">
-        <v>0.6</v>
+        <v>0.32</v>
       </c>
       <c r="F132" t="inlineStr">
         <is>
-          <t>closest</t>
+          <t>selfish</t>
         </is>
       </c>
     </row>
     <row r="133">
       <c r="A133" s="1" t="inlineStr">
         <is>
-          <t>-Mr4hi4w_fxN0OyW6Zn7</t>
+          <t>-Mr4Zi_Kuu8k4mSOXZS1</t>
         </is>
       </c>
       <c r="B133" t="n">
-        <v>-0.25</v>
+        <v>0.5</v>
       </c>
       <c r="C133" t="n">
-        <v>0.31</v>
+        <v>0.5</v>
       </c>
       <c r="D133" t="n">
-        <v>-0.15</v>
+        <v>0.6</v>
       </c>
       <c r="E133" t="n">
-        <v>0.46</v>
+        <v>0.65</v>
       </c>
       <c r="F133" t="inlineStr">
         <is>
@@ -3631,68 +3631,68 @@
     <row r="134">
       <c r="A134" s="1" t="inlineStr">
         <is>
-          <t>-Mr4hkgWqo_Aim6hCwar</t>
+          <t>-Mr4Zv2TnMWi8pXYaSPy</t>
         </is>
       </c>
       <c r="B134" t="n">
-        <v>-0.25</v>
+        <v>0.03</v>
       </c>
       <c r="C134" t="n">
-        <v>0.27</v>
+        <v>-0.04999999999999999</v>
       </c>
       <c r="D134" t="n">
-        <v>-0.2</v>
+        <v>0.03</v>
       </c>
       <c r="E134" t="n">
-        <v>0.47</v>
+        <v>0.2</v>
       </c>
       <c r="F134" t="inlineStr">
         <is>
-          <t>farthest</t>
+          <t>random</t>
         </is>
       </c>
     </row>
     <row r="135">
       <c r="A135" s="1" t="inlineStr">
         <is>
-          <t>-Mr4hp5SMdmQkBorGdP2</t>
+          <t>-Mr4Zw08vxDeIWifKmcp</t>
         </is>
       </c>
       <c r="B135" t="n">
-        <v>-0.76</v>
+        <v>0.4</v>
       </c>
       <c r="C135" t="n">
-        <v>0.18</v>
+        <v>0.4500000000000001</v>
       </c>
       <c r="D135" t="n">
-        <v>-0.66</v>
+        <v>0.55</v>
       </c>
       <c r="E135" t="n">
-        <v>0.33</v>
+        <v>0.55</v>
       </c>
       <c r="F135" t="inlineStr">
         <is>
-          <t>random</t>
+          <t>farthest</t>
         </is>
       </c>
     </row>
     <row r="136">
       <c r="A136" s="1" t="inlineStr">
         <is>
-          <t>-Mr4hrdY8etHamtTMUkU</t>
+          <t>-Mr4_-TKLRXbB1clPMdP</t>
         </is>
       </c>
       <c r="B136" t="n">
-        <v>-0.35</v>
+        <v>0.57</v>
       </c>
       <c r="C136" t="n">
-        <v>-0.8</v>
+        <v>0.4</v>
       </c>
       <c r="D136" t="n">
-        <v>-0.35</v>
+        <v>0.62</v>
       </c>
       <c r="E136" t="n">
-        <v>-0.55</v>
+        <v>0.6</v>
       </c>
       <c r="F136" t="inlineStr">
         <is>
@@ -3703,68 +3703,68 @@
     <row r="137">
       <c r="A137" s="1" t="inlineStr">
         <is>
-          <t>-Mr4iZa6QtFp83RQZDJZ</t>
+          <t>-Mr4_BrvGGJ1lAwDLl8r</t>
         </is>
       </c>
       <c r="B137" t="n">
-        <v>0.58</v>
+        <v>1.26</v>
       </c>
       <c r="C137" t="n">
-        <v>0.3799999999999999</v>
+        <v>0.35</v>
       </c>
       <c r="D137" t="n">
-        <v>0.63</v>
+        <v>1.26</v>
       </c>
       <c r="E137" t="n">
-        <v>0.58</v>
+        <v>0.6</v>
       </c>
       <c r="F137" t="inlineStr">
         <is>
-          <t>random</t>
+          <t>selfish</t>
         </is>
       </c>
     </row>
     <row r="138">
       <c r="A138" s="1" t="inlineStr">
         <is>
-          <t>-Mr4jSWTdYthHCNnEES8</t>
+          <t>-Mr4_GdddSEv1KVlneSH</t>
         </is>
       </c>
       <c r="B138" t="n">
-        <v>0.3</v>
+        <v>1.05</v>
       </c>
       <c r="C138" t="n">
-        <v>0.3</v>
+        <v>0.9999999999999999</v>
       </c>
       <c r="D138" t="n">
-        <v>0.35</v>
+        <v>1.15</v>
       </c>
       <c r="E138" t="n">
-        <v>0.5</v>
+        <v>1.15</v>
       </c>
       <c r="F138" t="inlineStr">
         <is>
-          <t>farthest</t>
+          <t>TSP</t>
         </is>
       </c>
     </row>
     <row r="139">
       <c r="A139" s="1" t="inlineStr">
         <is>
-          <t>-Mr4kVKNdGM29BXhdRZJ</t>
+          <t>-Mr4_ICrbKPcl3Cztxwb</t>
         </is>
       </c>
       <c r="B139" t="n">
-        <v>0.38</v>
+        <v>0.33</v>
       </c>
       <c r="C139" t="n">
-        <v>0.09999999999999998</v>
+        <v>0.57</v>
       </c>
       <c r="D139" t="n">
-        <v>0.48</v>
+        <v>0.43</v>
       </c>
       <c r="E139" t="n">
-        <v>0.25</v>
+        <v>0.72</v>
       </c>
       <c r="F139" t="inlineStr">
         <is>
@@ -3775,20 +3775,20 @@
     <row r="140">
       <c r="A140" s="1" t="inlineStr">
         <is>
-          <t>-Mr4kkZ3SHdgw489ERN3</t>
+          <t>-Mr4_ZKMOXNVUO6Qnjhb</t>
         </is>
       </c>
       <c r="B140" t="n">
-        <v>0.35</v>
+        <v>1.05</v>
       </c>
       <c r="C140" t="n">
-        <v>0.91</v>
+        <v>0.9999999999999999</v>
       </c>
       <c r="D140" t="n">
-        <v>0.5</v>
+        <v>1.15</v>
       </c>
       <c r="E140" t="n">
-        <v>1.01</v>
+        <v>1.15</v>
       </c>
       <c r="F140" t="inlineStr">
         <is>
@@ -3799,44 +3799,44 @@
     <row r="141">
       <c r="A141" s="1" t="inlineStr">
         <is>
-          <t>-Mr4ksHT9xaa-BlDDtDV</t>
+          <t>-Mr4_c1eWQi5mALBc8Vb</t>
         </is>
       </c>
       <c r="B141" t="n">
-        <v>0.85</v>
+        <v>-0.18</v>
       </c>
       <c r="C141" t="n">
-        <v>0.9700000000000001</v>
+        <v>-0.01999999999999999</v>
       </c>
       <c r="D141" t="n">
-        <v>1</v>
+        <v>-0.18</v>
       </c>
       <c r="E141" t="n">
-        <v>1.07</v>
+        <v>0.23</v>
       </c>
       <c r="F141" t="inlineStr">
         <is>
-          <t>closest</t>
+          <t>random</t>
         </is>
       </c>
     </row>
     <row r="142">
       <c r="A142" s="1" t="inlineStr">
         <is>
-          <t>-Mr4m4BJR_rHGhegppT7</t>
+          <t>-Mr4_pR7d8f5x1PRyHbt</t>
         </is>
       </c>
       <c r="B142" t="n">
-        <v>0.6799999999999999</v>
+        <v>0.52</v>
       </c>
       <c r="C142" t="n">
-        <v>0.4</v>
+        <v>0.29</v>
       </c>
       <c r="D142" t="n">
-        <v>0.73</v>
+        <v>0.52</v>
       </c>
       <c r="E142" t="n">
-        <v>0.6</v>
+        <v>0.54</v>
       </c>
       <c r="F142" t="inlineStr">
         <is>
@@ -3847,247 +3847,247 @@
     <row r="143">
       <c r="A143" s="1" t="inlineStr">
         <is>
-          <t>-Mr4mGCYLyotdd6lhJiS</t>
+          <t>-Mr4bNQJo1l3U7zrP2PJ</t>
         </is>
       </c>
       <c r="B143" t="n">
-        <v>0.75</v>
+        <v>-1.34</v>
       </c>
       <c r="C143" t="n">
-        <v>0.75</v>
+        <v>-1.5</v>
       </c>
       <c r="D143" t="n">
-        <v>0.85</v>
+        <v>-1.24</v>
       </c>
       <c r="E143" t="n">
-        <v>0.9</v>
+        <v>-1.35</v>
       </c>
       <c r="F143" t="inlineStr">
         <is>
-          <t>closest</t>
+          <t>farthest</t>
         </is>
       </c>
     </row>
     <row r="144">
       <c r="A144" s="1" t="inlineStr">
         <is>
-          <t>-Mr4mVFPRzarDuMNjtyR</t>
+          <t>-Mr4bWLBRG3475BpxIUJ</t>
         </is>
       </c>
       <c r="B144" t="n">
-        <v>0.41</v>
+        <v>0.7000000000000001</v>
       </c>
       <c r="C144" t="n">
-        <v>0.2</v>
+        <v>0.7</v>
       </c>
       <c r="D144" t="n">
-        <v>0.46</v>
+        <v>0.8</v>
       </c>
       <c r="E144" t="n">
-        <v>0.4</v>
+        <v>0.85</v>
       </c>
       <c r="F144" t="inlineStr">
         <is>
-          <t>random</t>
+          <t>closest</t>
         </is>
       </c>
     </row>
     <row r="145">
       <c r="A145" s="1" t="inlineStr">
         <is>
-          <t>-Mr4oBcWIAlIKyaxtCj_</t>
+          <t>-Mr4bY4JZ3gTh04PmI0D</t>
         </is>
       </c>
       <c r="B145" t="n">
-        <v>0.79</v>
+        <v>1</v>
       </c>
       <c r="C145" t="n">
-        <v>-0.17</v>
+        <v>0.9999999999999999</v>
       </c>
       <c r="D145" t="n">
-        <v>0.79</v>
+        <v>1.1</v>
       </c>
       <c r="E145" t="n">
-        <v>0.08</v>
+        <v>1.15</v>
       </c>
       <c r="F145" t="inlineStr">
         <is>
-          <t>selfish</t>
+          <t>TSP</t>
         </is>
       </c>
     </row>
     <row r="146">
       <c r="A146" s="1" t="inlineStr">
         <is>
-          <t>-Mr4ocz7UVAK56Iv8sfU</t>
+          <t>-Mr4d6kLpnPruwzbNjeh</t>
         </is>
       </c>
       <c r="B146" t="n">
-        <v>0.9</v>
+        <v>1.26</v>
       </c>
       <c r="C146" t="n">
-        <v>0.9</v>
+        <v>0.3</v>
       </c>
       <c r="D146" t="n">
-        <v>1</v>
+        <v>1.26</v>
       </c>
       <c r="E146" t="n">
-        <v>1.05</v>
+        <v>0.55</v>
       </c>
       <c r="F146" t="inlineStr">
         <is>
-          <t>TSP</t>
+          <t>selfish</t>
         </is>
       </c>
     </row>
     <row r="147">
       <c r="A147" s="1" t="inlineStr">
         <is>
-          <t>-Mr4olbjdQCovNCuANI-</t>
+          <t>-Mr4eWG-5xqB9Q6Dnmv3</t>
         </is>
       </c>
       <c r="B147" t="n">
-        <v>0.62</v>
+        <v>0.5499999999999999</v>
       </c>
       <c r="C147" t="n">
-        <v>0.3</v>
+        <v>0.79</v>
       </c>
       <c r="D147" t="n">
-        <v>0.62</v>
+        <v>0.7</v>
       </c>
       <c r="E147" t="n">
-        <v>0.55</v>
+        <v>0.89</v>
       </c>
       <c r="F147" t="inlineStr">
         <is>
-          <t>random</t>
+          <t>closest</t>
         </is>
       </c>
     </row>
     <row r="148">
       <c r="A148" s="1" t="inlineStr">
         <is>
-          <t>-Mr4p4Dn5PfCGODsa1nJ</t>
+          <t>-Mr4ej5yR8BD_KnrALKV</t>
         </is>
       </c>
       <c r="B148" t="n">
-        <v>0.7000000000000001</v>
+        <v>0.29</v>
       </c>
       <c r="C148" t="n">
-        <v>0.6899999999999999</v>
+        <v>0.29</v>
       </c>
       <c r="D148" t="n">
-        <v>0.8</v>
+        <v>0.39</v>
       </c>
       <c r="E148" t="n">
-        <v>0.84</v>
+        <v>0.44</v>
       </c>
       <c r="F148" t="inlineStr">
         <is>
-          <t>closest</t>
+          <t>random</t>
         </is>
       </c>
     </row>
     <row r="149">
       <c r="A149" s="1" t="inlineStr">
         <is>
-          <t>-Mr4pM-XfYBaivfXUe_i</t>
+          <t>-Mr4eseUbQr_kkfGoJiA</t>
         </is>
       </c>
       <c r="B149" t="n">
-        <v>1.18</v>
+        <v>0.7000000000000001</v>
       </c>
       <c r="C149" t="n">
-        <v>0</v>
+        <v>0.6899999999999999</v>
       </c>
       <c r="D149" t="n">
-        <v>1.18</v>
+        <v>0.8</v>
       </c>
       <c r="E149" t="n">
-        <v>0.25</v>
+        <v>0.84</v>
       </c>
       <c r="F149" t="inlineStr">
         <is>
-          <t>selfish</t>
+          <t>closest</t>
         </is>
       </c>
     </row>
     <row r="150">
       <c r="A150" s="1" t="inlineStr">
         <is>
-          <t>-Mr4pSsH2YJq06B8CIKz</t>
+          <t>-Mr4et1M31FSgHYxaXto</t>
         </is>
       </c>
       <c r="B150" t="n">
-        <v>1.17</v>
+        <v>0.66</v>
       </c>
       <c r="C150" t="n">
-        <v>-0.1</v>
+        <v>0.3</v>
       </c>
       <c r="D150" t="n">
-        <v>1.17</v>
+        <v>0.66</v>
       </c>
       <c r="E150" t="n">
-        <v>0.15</v>
+        <v>0.55</v>
       </c>
       <c r="F150" t="inlineStr">
         <is>
-          <t>selfish</t>
+          <t>random</t>
         </is>
       </c>
     </row>
     <row r="151">
       <c r="A151" s="1" t="inlineStr">
         <is>
-          <t>-Mr4paOlBK74VZ4Jl_sq</t>
+          <t>-Mr4eyZJx-gU5Cacgqq-</t>
         </is>
       </c>
       <c r="B151" t="n">
-        <v>0.5299999999999999</v>
+        <v>0.9500000000000001</v>
       </c>
       <c r="C151" t="n">
-        <v>0.09999999999999998</v>
+        <v>0.9500000000000001</v>
       </c>
       <c r="D151" t="n">
-        <v>0.58</v>
+        <v>1.05</v>
       </c>
       <c r="E151" t="n">
-        <v>0.3</v>
+        <v>1.1</v>
       </c>
       <c r="F151" t="inlineStr">
         <is>
-          <t>farthest</t>
+          <t>TSP</t>
         </is>
       </c>
     </row>
     <row r="152">
       <c r="A152" s="1" t="inlineStr">
         <is>
-          <t>-Mr4pnmKrpItABjVIBI9</t>
+          <t>-Mr4f3EUA-I93xEt4s-W</t>
         </is>
       </c>
       <c r="B152" t="n">
-        <v>0.25</v>
+        <v>0.8</v>
       </c>
       <c r="C152" t="n">
-        <v>0.3699999999999999</v>
+        <v>0.7</v>
       </c>
       <c r="D152" t="n">
-        <v>0.3</v>
+        <v>0.9</v>
       </c>
       <c r="E152" t="n">
-        <v>0.57</v>
+        <v>0.85</v>
       </c>
       <c r="F152" t="inlineStr">
         <is>
-          <t>farthest</t>
+          <t>closest</t>
         </is>
       </c>
     </row>
     <row r="153">
       <c r="A153" s="1" t="inlineStr">
         <is>
-          <t>-Mr4qSbuzfLx3fxlJkle</t>
+          <t>-Mr4f4NUS_ANE-GljaXl</t>
         </is>
       </c>
       <c r="B153" t="n">
@@ -4104,51 +4104,51 @@
       </c>
       <c r="F153" t="inlineStr">
         <is>
-          <t>TSP</t>
+          <t>closest</t>
         </is>
       </c>
     </row>
     <row r="154">
       <c r="A154" s="1" t="inlineStr">
         <is>
-          <t>-Mr4rJaXGFM8vM0T6I-d</t>
+          <t>-Mr4fBZl_62qSc_4RnDv</t>
         </is>
       </c>
       <c r="B154" t="n">
-        <v>0.4</v>
+        <v>1</v>
       </c>
       <c r="C154" t="n">
-        <v>0.48</v>
+        <v>0.9999999999999999</v>
       </c>
       <c r="D154" t="n">
-        <v>0.5</v>
+        <v>1.1</v>
       </c>
       <c r="E154" t="n">
-        <v>0.63</v>
+        <v>1.15</v>
       </c>
       <c r="F154" t="inlineStr">
         <is>
-          <t>closest</t>
+          <t>TSP</t>
         </is>
       </c>
     </row>
     <row r="155">
       <c r="A155" s="1" t="inlineStr">
         <is>
-          <t>-Mr4tlQ1MpDlTDqm6vlk</t>
+          <t>-Mr4fC9EkjHHPnr1zUd8</t>
         </is>
       </c>
       <c r="B155" t="n">
         <v>0.65</v>
       </c>
       <c r="C155" t="n">
-        <v>0.65</v>
+        <v>0.6</v>
       </c>
       <c r="D155" t="n">
         <v>0.75</v>
       </c>
       <c r="E155" t="n">
-        <v>0.8</v>
+        <v>0.75</v>
       </c>
       <c r="F155" t="inlineStr">
         <is>
@@ -4159,20 +4159,20 @@
     <row r="156">
       <c r="A156" s="1" t="inlineStr">
         <is>
-          <t>-Mr4vbl8s8DO0m_0HBwd</t>
+          <t>-Mr4fa-QIY2yVwGZExoD</t>
         </is>
       </c>
       <c r="B156" t="n">
-        <v>0.87</v>
+        <v>0.25</v>
       </c>
       <c r="C156" t="n">
-        <v>0.3</v>
+        <v>0.25</v>
       </c>
       <c r="D156" t="n">
-        <v>0.87</v>
+        <v>0.25</v>
       </c>
       <c r="E156" t="n">
-        <v>0.55</v>
+        <v>0.5</v>
       </c>
       <c r="F156" t="inlineStr">
         <is>
@@ -4183,20 +4183,20 @@
     <row r="157">
       <c r="A157" s="1" t="inlineStr">
         <is>
-          <t>-Mr4vpo0C7EkcFL08tgF</t>
+          <t>-Mr4ffBo8AxSYU6oNxDV</t>
         </is>
       </c>
       <c r="B157" t="n">
-        <v>0.3</v>
+        <v>1</v>
       </c>
       <c r="C157" t="n">
-        <v>0.25</v>
+        <v>0.9999999999999999</v>
       </c>
       <c r="D157" t="n">
-        <v>0.45</v>
+        <v>1.1</v>
       </c>
       <c r="E157" t="n">
-        <v>0.35</v>
+        <v>1.15</v>
       </c>
       <c r="F157" t="inlineStr">
         <is>
@@ -4207,116 +4207,116 @@
     <row r="158">
       <c r="A158" s="1" t="inlineStr">
         <is>
-          <t>-Mr5A5eDh_hZ_5aAChtI</t>
+          <t>-Mr4fiUqvTaGet47n6rF</t>
         </is>
       </c>
       <c r="B158" t="n">
-        <v>0.49</v>
+        <v>1.05</v>
       </c>
       <c r="C158" t="n">
-        <v>0.04999999999999999</v>
+        <v>0.9999999999999999</v>
       </c>
       <c r="D158" t="n">
-        <v>0.59</v>
+        <v>1.15</v>
       </c>
       <c r="E158" t="n">
-        <v>0.2</v>
+        <v>1.15</v>
       </c>
       <c r="F158" t="inlineStr">
         <is>
-          <t>random</t>
+          <t>TSP</t>
         </is>
       </c>
     </row>
     <row r="159">
       <c r="A159" s="1" t="inlineStr">
         <is>
-          <t>-Mr5BoE45Gn9AJJXjirU</t>
+          <t>-Mr4gAjnlvcW3RKZX703</t>
         </is>
       </c>
       <c r="B159" t="n">
-        <v>0.45</v>
+        <v>0.15</v>
       </c>
       <c r="C159" t="n">
-        <v>0.45</v>
+        <v>1.19</v>
       </c>
       <c r="D159" t="n">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="E159" t="n">
-        <v>0.65</v>
+        <v>1.24</v>
       </c>
       <c r="F159" t="inlineStr">
         <is>
-          <t>farthest</t>
+          <t>closest</t>
         </is>
       </c>
     </row>
     <row r="160">
       <c r="A160" s="1" t="inlineStr">
         <is>
-          <t>-Mr5TMSq5ynTUJE5agP6</t>
+          <t>-Mr4gIM5ATsxVHYlUnPm</t>
         </is>
       </c>
       <c r="B160" t="n">
-        <v>0.4</v>
+        <v>1.22</v>
       </c>
       <c r="C160" t="n">
-        <v>0.2</v>
+        <v>0.22</v>
       </c>
       <c r="D160" t="n">
-        <v>0.5</v>
+        <v>1.22</v>
       </c>
       <c r="E160" t="n">
-        <v>0.35</v>
+        <v>0.47</v>
       </c>
       <c r="F160" t="inlineStr">
         <is>
-          <t>farthest</t>
+          <t>selfish</t>
         </is>
       </c>
     </row>
     <row r="161">
       <c r="A161" s="1" t="inlineStr">
         <is>
-          <t>-Mr5gp9WxLYDKJXvYNWj</t>
+          <t>-Mr4gM9iXWa0OxaNz9pd</t>
         </is>
       </c>
       <c r="B161" t="n">
-        <v>0.25</v>
+        <v>1.26</v>
       </c>
       <c r="C161" t="n">
-        <v>0.4</v>
+        <v>0.35</v>
       </c>
       <c r="D161" t="n">
-        <v>0.35</v>
+        <v>1.26</v>
       </c>
       <c r="E161" t="n">
-        <v>0.55</v>
+        <v>0.6</v>
       </c>
       <c r="F161" t="inlineStr">
         <is>
-          <t>farthest</t>
+          <t>selfish</t>
         </is>
       </c>
     </row>
     <row r="162">
       <c r="A162" s="1" t="inlineStr">
         <is>
-          <t>-Mr6Fw-yi6Ld2xKNzu03</t>
+          <t>-Mr4gnhvp8zu4hyKSHT8</t>
         </is>
       </c>
       <c r="B162" t="n">
-        <v>0.25</v>
+        <v>1</v>
       </c>
       <c r="C162" t="n">
-        <v>1.25</v>
+        <v>0.9999999999999999</v>
       </c>
       <c r="D162" t="n">
-        <v>0.5</v>
+        <v>1.1</v>
       </c>
       <c r="E162" t="n">
-        <v>1.25</v>
+        <v>1.15</v>
       </c>
       <c r="F162" t="inlineStr">
         <is>
@@ -4327,672 +4327,888 @@
     <row r="163">
       <c r="A163" s="1" t="inlineStr">
         <is>
-          <t>-MrdFer4gDRv926_ks_a</t>
+          <t>-Mr4gppr7Vw6iIfcH6fv</t>
         </is>
       </c>
       <c r="B163" t="n">
-        <v>1.2</v>
+        <v>0</v>
       </c>
       <c r="C163" t="n">
+        <v>0</v>
+      </c>
+      <c r="D163" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="E163" t="n">
         <v>0.2</v>
       </c>
-      <c r="D163" t="n">
-        <v>1.2</v>
-      </c>
-      <c r="E163" t="n">
-        <v>0.45</v>
-      </c>
       <c r="F163" t="inlineStr">
         <is>
-          <t>ddqn distribution</t>
+          <t>farthest</t>
         </is>
       </c>
     </row>
     <row r="164">
       <c r="A164" s="1" t="inlineStr">
         <is>
-          <t>-MrdFg2YluAkff9volJO</t>
+          <t>-Mr4grc_XL69ykWx-MHR</t>
         </is>
       </c>
       <c r="B164" t="n">
-        <v>1.12</v>
+        <v>0.5</v>
       </c>
       <c r="C164" t="n">
-        <v>0.9999999999999999</v>
+        <v>0.5</v>
       </c>
       <c r="D164" t="n">
-        <v>1.22</v>
+        <v>0.65</v>
       </c>
       <c r="E164" t="n">
-        <v>1.15</v>
+        <v>0.6</v>
       </c>
       <c r="F164" t="inlineStr">
         <is>
-          <t>sarl ddqn distribution</t>
+          <t>closest</t>
         </is>
       </c>
     </row>
     <row r="165">
       <c r="A165" s="1" t="inlineStr">
         <is>
-          <t>-MrdFlrPsNbJ2N0qRxa3</t>
+          <t>-Mr4hCX2_mf23fh_HfHD</t>
         </is>
       </c>
       <c r="B165" t="n">
-        <v>1.5</v>
+        <v>0.65</v>
       </c>
       <c r="C165" t="n">
-        <v>-0.26</v>
+        <v>0.64</v>
       </c>
       <c r="D165" t="n">
-        <v>1.5</v>
+        <v>0.8</v>
       </c>
       <c r="E165" t="n">
-        <v>-0.01</v>
+        <v>0.74</v>
       </c>
       <c r="F165" t="inlineStr">
         <is>
-          <t>sarl ddqn distribution</t>
+          <t>closest</t>
         </is>
       </c>
     </row>
     <row r="166">
       <c r="A166" s="1" t="inlineStr">
         <is>
-          <t>-MrdFqxW17UgmS4HzTe9</t>
+          <t>-Mr4hOoZjliyARNml8Tv</t>
         </is>
       </c>
       <c r="B166" t="n">
-        <v>1.1</v>
+        <v>0.45</v>
       </c>
       <c r="C166" t="n">
-        <v>0.9</v>
+        <v>0.45</v>
       </c>
       <c r="D166" t="n">
-        <v>1.2</v>
+        <v>0.5</v>
       </c>
       <c r="E166" t="n">
-        <v>1.05</v>
+        <v>0.65</v>
       </c>
       <c r="F166" t="inlineStr">
         <is>
-          <t>sarl ddqn distribution</t>
+          <t>farthest</t>
         </is>
       </c>
     </row>
     <row r="167">
       <c r="A167" s="1" t="inlineStr">
         <is>
-          <t>-MrdFwXN2alRSW76kUXP</t>
+          <t>-Mr4hSrulYrbm5UIrKMF</t>
         </is>
       </c>
       <c r="B167" t="n">
-        <v>1.12</v>
+        <v>0.55</v>
       </c>
       <c r="C167" t="n">
-        <v>0.9999999999999999</v>
+        <v>0.71</v>
       </c>
       <c r="D167" t="n">
-        <v>1.22</v>
+        <v>0.75</v>
       </c>
       <c r="E167" t="n">
-        <v>1.15</v>
+        <v>0.76</v>
       </c>
       <c r="F167" t="inlineStr">
         <is>
-          <t>sarl ddqn distribution</t>
+          <t>TSP</t>
         </is>
       </c>
     </row>
     <row r="168">
       <c r="A168" s="1" t="inlineStr">
         <is>
-          <t>-MrdFyacMZhdEI9MjDca</t>
+          <t>-Mr4hYkL43oy86Glh53W</t>
         </is>
       </c>
       <c r="B168" t="n">
-        <v>1.18</v>
+        <v>0.5</v>
       </c>
       <c r="C168" t="n">
-        <v>0.15</v>
+        <v>0.5</v>
       </c>
       <c r="D168" t="n">
-        <v>1.18</v>
+        <v>0.65</v>
       </c>
       <c r="E168" t="n">
-        <v>0.4</v>
+        <v>0.6</v>
       </c>
       <c r="F168" t="inlineStr">
         <is>
-          <t>ddqn distribution</t>
+          <t>closest</t>
         </is>
       </c>
     </row>
     <row r="169">
       <c r="A169" s="1" t="inlineStr">
         <is>
-          <t>-MrdFyakM7hyP7JM9c32</t>
+          <t>-Mr4hi4w_fxN0OyW6Zn7</t>
         </is>
       </c>
       <c r="B169" t="n">
-        <v>1.14</v>
+        <v>-0.25</v>
       </c>
       <c r="C169" t="n">
-        <v>-0.1</v>
+        <v>0.31</v>
       </c>
       <c r="D169" t="n">
-        <v>1.14</v>
+        <v>-0.15</v>
       </c>
       <c r="E169" t="n">
-        <v>0.15</v>
+        <v>0.46</v>
       </c>
       <c r="F169" t="inlineStr">
         <is>
-          <t>ddqn distribution</t>
+          <t>farthest</t>
         </is>
       </c>
     </row>
     <row r="170">
       <c r="A170" s="1" t="inlineStr">
         <is>
-          <t>-MrdG1VmAbRHmN_niOws</t>
+          <t>-Mr4hkgWqo_Aim6hCwar</t>
         </is>
       </c>
       <c r="B170" t="n">
-        <v>1.5</v>
+        <v>-0.25</v>
       </c>
       <c r="C170" t="n">
-        <v>-0.01999999999999999</v>
+        <v>0.27</v>
       </c>
       <c r="D170" t="n">
-        <v>1.5</v>
+        <v>-0.2</v>
       </c>
       <c r="E170" t="n">
-        <v>0.23</v>
+        <v>0.47</v>
       </c>
       <c r="F170" t="inlineStr">
         <is>
-          <t>sarl ddqn distribution</t>
+          <t>farthest</t>
         </is>
       </c>
     </row>
     <row r="171">
       <c r="A171" s="1" t="inlineStr">
         <is>
-          <t>-MrdG3NfK25v98pteegm</t>
+          <t>-Mr4hp5SMdmQkBorGdP2</t>
         </is>
       </c>
       <c r="B171" t="n">
-        <v>1.1</v>
+        <v>-0.76</v>
       </c>
       <c r="C171" t="n">
-        <v>0.9</v>
+        <v>0.18</v>
       </c>
       <c r="D171" t="n">
-        <v>1.2</v>
+        <v>-0.66</v>
       </c>
       <c r="E171" t="n">
-        <v>1.05</v>
+        <v>0.33</v>
       </c>
       <c r="F171" t="inlineStr">
         <is>
-          <t>sarl ddqn distribution</t>
+          <t>random</t>
         </is>
       </c>
     </row>
     <row r="172">
       <c r="A172" s="1" t="inlineStr">
         <is>
-          <t>-MrdGdPyXV8E9KnNwdeX</t>
+          <t>-Mr4hrdY8etHamtTMUkU</t>
         </is>
       </c>
       <c r="B172" t="n">
-        <v>1.5</v>
+        <v>-0.35</v>
       </c>
       <c r="C172" t="n">
-        <v>-0.1</v>
+        <v>-0.8</v>
       </c>
       <c r="D172" t="n">
-        <v>1.5</v>
+        <v>-0.35</v>
       </c>
       <c r="E172" t="n">
-        <v>0.15</v>
+        <v>-0.55</v>
       </c>
       <c r="F172" t="inlineStr">
         <is>
-          <t>sarl ddqn distribution</t>
+          <t>random</t>
         </is>
       </c>
     </row>
     <row r="173">
       <c r="A173" s="1" t="inlineStr">
         <is>
-          <t>-MrdGgeKl0L2xLaxxJqb</t>
+          <t>-Mr4iZa6QtFp83RQZDJZ</t>
         </is>
       </c>
       <c r="B173" t="n">
-        <v>1.1</v>
+        <v>0.58</v>
       </c>
       <c r="C173" t="n">
-        <v>0.9</v>
+        <v>0.3799999999999999</v>
       </c>
       <c r="D173" t="n">
-        <v>1.2</v>
+        <v>0.63</v>
       </c>
       <c r="E173" t="n">
-        <v>1.05</v>
+        <v>0.58</v>
       </c>
       <c r="F173" t="inlineStr">
         <is>
-          <t>sarl ddqn distribution</t>
+          <t>random</t>
         </is>
       </c>
     </row>
     <row r="174">
       <c r="A174" s="1" t="inlineStr">
         <is>
-          <t>-MrdGi5MLcwnRJ1Jf9-H</t>
+          <t>-Mr4jSWTdYthHCNnEES8</t>
         </is>
       </c>
       <c r="B174" t="n">
-        <v>1.1</v>
+        <v>0.3</v>
       </c>
       <c r="C174" t="n">
-        <v>-0.25</v>
+        <v>0.3</v>
       </c>
       <c r="D174" t="n">
-        <v>1.1</v>
+        <v>0.35</v>
       </c>
       <c r="E174" t="n">
-        <v>-0</v>
+        <v>0.5</v>
       </c>
       <c r="F174" t="inlineStr">
         <is>
-          <t>ddqn distribution</t>
+          <t>farthest</t>
         </is>
       </c>
     </row>
     <row r="175">
       <c r="A175" s="1" t="inlineStr">
         <is>
-          <t>-MrdHFs2YjBk1CHz5irF</t>
+          <t>-Mr4k1vylLWl-e3RBknX</t>
         </is>
       </c>
       <c r="B175" t="n">
-        <v>0.8300000000000001</v>
+        <v>0.55</v>
       </c>
       <c r="C175" t="n">
-        <v>0.4</v>
+        <v>0.35</v>
       </c>
       <c r="D175" t="n">
-        <v>0.93</v>
+        <v>0.65</v>
       </c>
       <c r="E175" t="n">
-        <v>0.55</v>
+        <v>0.5</v>
       </c>
       <c r="F175" t="inlineStr">
         <is>
-          <t>sarl ddqn distribution</t>
+          <t>random</t>
         </is>
       </c>
     </row>
     <row r="176">
       <c r="A176" s="1" t="inlineStr">
         <is>
-          <t>-MrdHf-9y2xF6XfkrQZD</t>
+          <t>-Mr4kVKNdGM29BXhdRZJ</t>
         </is>
       </c>
       <c r="B176" t="n">
-        <v>1.21</v>
+        <v>0.38</v>
       </c>
       <c r="C176" t="n">
+        <v>0.09999999999999998</v>
+      </c>
+      <c r="D176" t="n">
+        <v>0.48</v>
+      </c>
+      <c r="E176" t="n">
         <v>0.25</v>
       </c>
-      <c r="D176" t="n">
-        <v>1.21</v>
-      </c>
-      <c r="E176" t="n">
-        <v>0.5</v>
-      </c>
       <c r="F176" t="inlineStr">
         <is>
-          <t>ddqn distribution</t>
+          <t>random</t>
         </is>
       </c>
     </row>
     <row r="177">
       <c r="A177" s="1" t="inlineStr">
         <is>
-          <t>-MrdIdVpblIi_ehLzWjg</t>
+          <t>-Mr4kkZ3SHdgw489ERN3</t>
         </is>
       </c>
       <c r="B177" t="n">
-        <v>1.11</v>
+        <v>0.35</v>
       </c>
       <c r="C177" t="n">
-        <v>-0.25</v>
+        <v>0.91</v>
       </c>
       <c r="D177" t="n">
-        <v>1.11</v>
+        <v>0.5</v>
       </c>
       <c r="E177" t="n">
-        <v>-0</v>
+        <v>1.01</v>
       </c>
       <c r="F177" t="inlineStr">
         <is>
-          <t>ddqn distribution</t>
+          <t>TSP</t>
         </is>
       </c>
     </row>
     <row r="178">
       <c r="A178" s="1" t="inlineStr">
         <is>
-          <t>-MrdIoLv0ad6E3HFBV97</t>
+          <t>-Mr4ksHT9xaa-BlDDtDV</t>
         </is>
       </c>
       <c r="B178" t="n">
-        <v>1.05</v>
+        <v>0.85</v>
       </c>
       <c r="C178" t="n">
-        <v>-0.5</v>
+        <v>0.9700000000000001</v>
       </c>
       <c r="D178" t="n">
-        <v>1.05</v>
+        <v>1</v>
       </c>
       <c r="E178" t="n">
-        <v>-0.25</v>
+        <v>1.07</v>
       </c>
       <c r="F178" t="inlineStr">
         <is>
-          <t>ddqn distribution</t>
+          <t>closest</t>
         </is>
       </c>
     </row>
     <row r="179">
       <c r="A179" s="1" t="inlineStr">
         <is>
-          <t>-MrdJZ6eMdyvYvc5I9QF</t>
+          <t>-Mr4m4BJR_rHGhegppT7</t>
         </is>
       </c>
       <c r="B179" t="n">
-        <v>0.59</v>
+        <v>0.6799999999999999</v>
       </c>
       <c r="C179" t="n">
-        <v>-1.25</v>
+        <v>0.4</v>
       </c>
       <c r="D179" t="n">
-        <v>0.64</v>
+        <v>0.73</v>
       </c>
       <c r="E179" t="n">
-        <v>-1.05</v>
+        <v>0.6</v>
       </c>
       <c r="F179" t="inlineStr">
         <is>
-          <t>ddqn distribution</t>
+          <t>random</t>
         </is>
       </c>
     </row>
     <row r="180">
       <c r="A180" s="1" t="inlineStr">
         <is>
-          <t>-MrdKnJb85CwzDlTBYi-</t>
+          <t>-Mr4mGCYLyotdd6lhJiS</t>
         </is>
       </c>
       <c r="B180" t="n">
-        <v>1.02</v>
+        <v>0.75</v>
       </c>
       <c r="C180" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="D180" t="n">
+        <v>0.85</v>
+      </c>
+      <c r="E180" t="n">
         <v>0.9</v>
       </c>
-      <c r="D180" t="n">
-        <v>1.12</v>
-      </c>
-      <c r="E180" t="n">
-        <v>1.05</v>
-      </c>
       <c r="F180" t="inlineStr">
         <is>
-          <t>sarl ddqn distribution</t>
+          <t>closest</t>
         </is>
       </c>
     </row>
     <row r="181">
       <c r="A181" s="1" t="inlineStr">
         <is>
-          <t>-MrdLDQDnifFLU8_MEmZ</t>
+          <t>-Mr4mVFPRzarDuMNjtyR</t>
         </is>
       </c>
       <c r="B181" t="n">
-        <v>1.12</v>
+        <v>0.41</v>
       </c>
       <c r="C181" t="n">
-        <v>0.9999999999999999</v>
+        <v>0.2</v>
       </c>
       <c r="D181" t="n">
-        <v>1.22</v>
+        <v>0.46</v>
       </c>
       <c r="E181" t="n">
-        <v>1.15</v>
+        <v>0.4</v>
       </c>
       <c r="F181" t="inlineStr">
         <is>
-          <t>sarl ddqn distribution</t>
+          <t>random</t>
         </is>
       </c>
     </row>
     <row r="182">
       <c r="A182" s="1" t="inlineStr">
         <is>
-          <t>-MrdLcZZcDzbRKfQFigP</t>
+          <t>-Mr4oBcWIAlIKyaxtCj_</t>
         </is>
       </c>
       <c r="B182" t="n">
-        <v>0.99</v>
+        <v>0.79</v>
       </c>
       <c r="C182" t="n">
-        <v>-0.23</v>
+        <v>-0.17</v>
       </c>
       <c r="D182" t="n">
-        <v>1.04</v>
+        <v>0.79</v>
       </c>
       <c r="E182" t="n">
-        <v>-0.03</v>
+        <v>0.08</v>
       </c>
       <c r="F182" t="inlineStr">
         <is>
-          <t>ddqn distribution</t>
+          <t>selfish</t>
         </is>
       </c>
     </row>
     <row r="183">
       <c r="A183" s="1" t="inlineStr">
         <is>
-          <t>-MrdMMhpRvOMbCEPCnE9</t>
+          <t>-Mr4ocz7UVAK56Iv8sfU</t>
         </is>
       </c>
       <c r="B183" t="n">
-        <v>1.12</v>
+        <v>0.9</v>
       </c>
       <c r="C183" t="n">
-        <v>0.9999999999999999</v>
+        <v>0.9</v>
       </c>
       <c r="D183" t="n">
-        <v>1.22</v>
+        <v>1</v>
       </c>
       <c r="E183" t="n">
-        <v>1.15</v>
+        <v>1.05</v>
       </c>
       <c r="F183" t="inlineStr">
         <is>
-          <t>sarl ddqn distribution</t>
+          <t>TSP</t>
         </is>
       </c>
     </row>
     <row r="184">
       <c r="A184" s="1" t="inlineStr">
         <is>
-          <t>-MrdMNhv5g13sn7iycXM</t>
+          <t>-Mr4olbjdQCovNCuANI-</t>
         </is>
       </c>
       <c r="B184" t="n">
-        <v>0.97</v>
+        <v>0.62</v>
       </c>
       <c r="C184" t="n">
-        <v>0.04999999999999999</v>
+        <v>0.3</v>
       </c>
       <c r="D184" t="n">
-        <v>1.02</v>
+        <v>0.62</v>
       </c>
       <c r="E184" t="n">
-        <v>0.25</v>
+        <v>0.55</v>
       </c>
       <c r="F184" t="inlineStr">
         <is>
-          <t>ddqn distribution</t>
+          <t>random</t>
         </is>
       </c>
     </row>
     <row r="185">
       <c r="A185" s="1" t="inlineStr">
         <is>
-          <t>-MrdOC_mRdUGKHE4tR-H</t>
+          <t>-Mr4p4Dn5PfCGODsa1nJ</t>
         </is>
       </c>
       <c r="B185" t="n">
-        <v>1.25</v>
+        <v>0.7000000000000001</v>
       </c>
       <c r="C185" t="n">
-        <v>0.29</v>
+        <v>0.6899999999999999</v>
       </c>
       <c r="D185" t="n">
-        <v>1.25</v>
+        <v>0.8</v>
       </c>
       <c r="E185" t="n">
-        <v>0.54</v>
+        <v>0.84</v>
       </c>
       <c r="F185" t="inlineStr">
         <is>
-          <t>ddqn distribution</t>
+          <t>closest</t>
         </is>
       </c>
     </row>
     <row r="186">
       <c r="A186" s="1" t="inlineStr">
         <is>
-          <t>-MrdOcWo2GsKlOqJJP6p</t>
+          <t>-Mr4pM-XfYBaivfXUe_i</t>
         </is>
       </c>
       <c r="B186" t="n">
         <v>1.18</v>
       </c>
       <c r="C186" t="n">
-        <v>-0.1</v>
+        <v>0</v>
       </c>
       <c r="D186" t="n">
         <v>1.18</v>
       </c>
       <c r="E186" t="n">
-        <v>0.15</v>
+        <v>0.25</v>
       </c>
       <c r="F186" t="inlineStr">
         <is>
-          <t>ddqn distribution</t>
+          <t>selfish</t>
         </is>
       </c>
     </row>
     <row r="187">
       <c r="A187" s="1" t="inlineStr">
         <is>
-          <t>-MrdPi-CK3L-Uom2bRBq</t>
+          <t>-Mr4pSsH2YJq06B8CIKz</t>
         </is>
       </c>
       <c r="B187" t="n">
-        <v>1.01</v>
+        <v>1.17</v>
       </c>
       <c r="C187" t="n">
-        <v>-0.06</v>
+        <v>-0.1</v>
       </c>
       <c r="D187" t="n">
-        <v>1.06</v>
+        <v>1.17</v>
       </c>
       <c r="E187" t="n">
-        <v>0.14</v>
+        <v>0.15</v>
       </c>
       <c r="F187" t="inlineStr">
         <is>
-          <t>ddqn distribution</t>
+          <t>selfish</t>
         </is>
       </c>
     </row>
     <row r="188">
       <c r="A188" s="1" t="inlineStr">
         <is>
-          <t>-MrdV17r27tPlQu_ufLf</t>
+          <t>-Mr4paOlBK74VZ4Jl_sq</t>
         </is>
       </c>
       <c r="B188" t="n">
-        <v>0.9600000000000001</v>
+        <v>0.5299999999999999</v>
       </c>
       <c r="C188" t="n">
-        <v>0.28</v>
+        <v>0.09999999999999998</v>
       </c>
       <c r="D188" t="n">
-        <v>1.06</v>
+        <v>0.58</v>
       </c>
       <c r="E188" t="n">
-        <v>0.43</v>
+        <v>0.3</v>
       </c>
       <c r="F188" t="inlineStr">
         <is>
-          <t>sarl ddqn distribution</t>
+          <t>farthest</t>
         </is>
       </c>
     </row>
     <row r="189">
       <c r="A189" s="1" t="inlineStr">
         <is>
-          <t>-MrdXE4yDuiCkRU9sFyO</t>
+          <t>-Mr4pnmKrpItABjVIBI9</t>
         </is>
       </c>
       <c r="B189" t="n">
-        <v>1.1</v>
+        <v>0.25</v>
       </c>
       <c r="C189" t="n">
-        <v>0.9</v>
+        <v>0.3699999999999999</v>
       </c>
       <c r="D189" t="n">
-        <v>1.2</v>
+        <v>0.3</v>
       </c>
       <c r="E189" t="n">
-        <v>1.05</v>
+        <v>0.57</v>
       </c>
       <c r="F189" t="inlineStr">
         <is>
-          <t>sarl ddqn distribution</t>
+          <t>farthest</t>
         </is>
       </c>
     </row>
     <row r="190">
       <c r="A190" s="1" t="inlineStr">
         <is>
-          <t>-MrdeUAfhVRV_uSeag7d</t>
+          <t>-Mr4qSbuzfLx3fxlJkle</t>
         </is>
       </c>
       <c r="B190" t="n">
-        <v>0.6</v>
+        <v>0.55</v>
       </c>
       <c r="C190" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="D190" t="n">
+        <v>0.65</v>
+      </c>
+      <c r="E190" t="n">
+        <v>0.65</v>
+      </c>
+      <c r="F190" t="inlineStr">
+        <is>
+          <t>TSP</t>
+        </is>
+      </c>
+    </row>
+    <row r="191">
+      <c r="A191" s="1" t="inlineStr">
+        <is>
+          <t>-Mr4rJaXGFM8vM0T6I-d</t>
+        </is>
+      </c>
+      <c r="B191" t="n">
         <v>0.4</v>
       </c>
-      <c r="D190" t="n">
+      <c r="C191" t="n">
+        <v>0.48</v>
+      </c>
+      <c r="D191" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="E191" t="n">
+        <v>0.63</v>
+      </c>
+      <c r="F191" t="inlineStr">
+        <is>
+          <t>closest</t>
+        </is>
+      </c>
+    </row>
+    <row r="192">
+      <c r="A192" s="1" t="inlineStr">
+        <is>
+          <t>-Mr4tlQ1MpDlTDqm6vlk</t>
+        </is>
+      </c>
+      <c r="B192" t="n">
+        <v>0.65</v>
+      </c>
+      <c r="C192" t="n">
+        <v>0.65</v>
+      </c>
+      <c r="D192" t="n">
         <v>0.75</v>
       </c>
-      <c r="E190" t="n">
+      <c r="E192" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="F192" t="inlineStr">
+        <is>
+          <t>closest</t>
+        </is>
+      </c>
+    </row>
+    <row r="193">
+      <c r="A193" s="1" t="inlineStr">
+        <is>
+          <t>-Mr4vbl8s8DO0m_0HBwd</t>
+        </is>
+      </c>
+      <c r="B193" t="n">
+        <v>0.87</v>
+      </c>
+      <c r="C193" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="D193" t="n">
+        <v>0.87</v>
+      </c>
+      <c r="E193" t="n">
+        <v>0.55</v>
+      </c>
+      <c r="F193" t="inlineStr">
+        <is>
+          <t>random</t>
+        </is>
+      </c>
+    </row>
+    <row r="194">
+      <c r="A194" s="1" t="inlineStr">
+        <is>
+          <t>-Mr4vpo0C7EkcFL08tgF</t>
+        </is>
+      </c>
+      <c r="B194" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="C194" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="D194" t="n">
+        <v>0.45</v>
+      </c>
+      <c r="E194" t="n">
+        <v>0.35</v>
+      </c>
+      <c r="F194" t="inlineStr">
+        <is>
+          <t>TSP</t>
+        </is>
+      </c>
+    </row>
+    <row r="195">
+      <c r="A195" s="1" t="inlineStr">
+        <is>
+          <t>-Mr5A5eDh_hZ_5aAChtI</t>
+        </is>
+      </c>
+      <c r="B195" t="n">
+        <v>0.49</v>
+      </c>
+      <c r="C195" t="n">
+        <v>0.04999999999999999</v>
+      </c>
+      <c r="D195" t="n">
+        <v>0.59</v>
+      </c>
+      <c r="E195" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="F195" t="inlineStr">
+        <is>
+          <t>random</t>
+        </is>
+      </c>
+    </row>
+    <row r="196">
+      <c r="A196" s="1" t="inlineStr">
+        <is>
+          <t>-Mr5BoE45Gn9AJJXjirU</t>
+        </is>
+      </c>
+      <c r="B196" t="n">
+        <v>0.45</v>
+      </c>
+      <c r="C196" t="n">
+        <v>0.45</v>
+      </c>
+      <c r="D196" t="n">
         <v>0.5</v>
       </c>
-      <c r="F190" t="inlineStr">
-        <is>
-          <t>sarl ddqn distribution</t>
+      <c r="E196" t="n">
+        <v>0.65</v>
+      </c>
+      <c r="F196" t="inlineStr">
+        <is>
+          <t>farthest</t>
+        </is>
+      </c>
+    </row>
+    <row r="197">
+      <c r="A197" s="1" t="inlineStr">
+        <is>
+          <t>-Mr5TMSq5ynTUJE5agP6</t>
+        </is>
+      </c>
+      <c r="B197" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="C197" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="D197" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="E197" t="n">
+        <v>0.35</v>
+      </c>
+      <c r="F197" t="inlineStr">
+        <is>
+          <t>farthest</t>
+        </is>
+      </c>
+    </row>
+    <row r="198">
+      <c r="A198" s="1" t="inlineStr">
+        <is>
+          <t>-Mr5gp9WxLYDKJXvYNWj</t>
+        </is>
+      </c>
+      <c r="B198" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="C198" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="D198" t="n">
+        <v>0.35</v>
+      </c>
+      <c r="E198" t="n">
+        <v>0.55</v>
+      </c>
+      <c r="F198" t="inlineStr">
+        <is>
+          <t>farthest</t>
+        </is>
+      </c>
+    </row>
+    <row r="199">
+      <c r="A199" s="1" t="inlineStr">
+        <is>
+          <t>-Mr6Fw-yi6Ld2xKNzu03</t>
+        </is>
+      </c>
+      <c r="B199" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="C199" t="n">
+        <v>1.25</v>
+      </c>
+      <c r="D199" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="E199" t="n">
+        <v>1.25</v>
+      </c>
+      <c r="F199" t="inlineStr">
+        <is>
+          <t>TSP</t>
         </is>
       </c>
     </row>

</xml_diff>